<commit_message>
Auto update Combined.xlsx [Sun Feb 15 16:21:24 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -455,7 +455,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Posting_Date</t>
+          <t>Deadline</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -479,7 +479,7 @@
       <c r="D2" s="1" t="inlineStr"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>02/04/2026</t>
+          <t>02/19/2026, 04:59 AM</t>
         </is>
       </c>
       <c r="F2" s="1">

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Mon Feb 16 04:21:52 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,18 +684,18 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1609019/ausbau-erneuerbarer-energien-expansion-of-renewable-energies", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1609019/ausbau-erneuerbarer-energien-expansion-of-renewable-energies", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
@@ -741,7 +741,7 @@
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
@@ -764,7 +764,7 @@
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
@@ -787,7 +787,7 @@
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -799,18 +799,18 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -822,18 +822,18 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -845,18 +845,18 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -868,18 +868,18 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -891,18 +891,18 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -914,18 +914,18 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
@@ -948,7 +948,7 @@
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -983,18 +983,18 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
+          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
+          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1029,18 +1029,18 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
+          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1052,18 +1052,18 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1075,18 +1075,18 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1098,18 +1098,18 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1121,18 +1121,18 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
+          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1144,18 +1144,18 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1167,18 +1167,18 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1190,18 +1190,18 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
+          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1213,18 +1213,18 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
+          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1236,18 +1236,18 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1259,18 +1259,18 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1282,18 +1282,18 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
+          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1305,18 +1305,18 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
+          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1328,18 +1328,18 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
+          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1351,18 +1351,18 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
+          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1374,18 +1374,18 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
+          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1397,18 +1397,18 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
+          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1443,18 +1443,18 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1466,18 +1466,18 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1489,18 +1489,18 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
+          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1512,18 +1512,18 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1535,18 +1535,18 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1558,18 +1558,18 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
+          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1581,18 +1581,18 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
+          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1604,18 +1604,18 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
+          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Safety, Climate</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1627,18 +1627,18 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
+          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1650,18 +1650,18 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
+          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1696,18 +1696,18 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including WTP of 6.0 MLD and STP of 3.5, 1.5 MLD, for Rangpo including O&amp;M for 5 years</t>
+          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448434/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works, including WTP 4.0, MLD and STP 1.5 MLD, for Pakyong including O&amp;M for 5 years</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including WTP of 6.0 MLD and STP of 3.5, 1.5 MLD, for Rangpo including O&amp;M for 5 years</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448435/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448434/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including STP of 2.5 MLD, for Singtam including O&amp;M for 5 years</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works, including WTP 4.0, MLD and STP 1.5 MLD, for Pakyong including O&amp;M for 5 years</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448436/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448435/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Bongaigaon/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Bongaigaon Town in Assam</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including STP of 2.5 MLD, for Singtam including O&amp;M for 5 years</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1445726/57262-ind-assam-urban-sector-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448436/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Goalpara/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Goalpara Town in Assam</t>
+          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Bongaigaon/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Bongaigaon Town in Assam</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1418982/57262-ind-assam-urban-sector-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1445726/57262-ind-assam-urban-sector-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Barpeta/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Barpeta Town in Assam</t>
+          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Goalpara/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Goalpara Town in Assam</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404713/57262-ind-assam-urban-sector-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1418982/57262-ind-assam-urban-sector-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Nalbari/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Nalbari Town in Assam</t>
+          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Barpeta/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Barpeta Town in Assam</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404712/57262-ind-assam-urban-sector-development-project", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404713/57262-ind-assam-urban-sector-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1857,18 +1857,18 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>Inclusive, Resilient, and Sustainable Housing for Urban Poor Sector Project in Tamil Nadu: Development of three Working Women Hostels (St. Thomas Mount, Hosur, and Thiruvanamalai) by Tamil Nadu Working Women's Hostels Corporation Limited (53067-004)</t>
+          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Nalbari/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Nalbari Town in Assam</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606477/inclusive-resilient-and-sustainable-housing-for-urban-poor-sector-project-in-tamil-nadu-development", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404712/57262-ind-assam-urban-sector-development-project", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1880,18 +1880,18 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>Information gathering and confirmation survey on AI human resource development and ecosystem formation for the global South (QCBS-lump sum type)</t>
+          <t>Inclusive, Resilient, and Sustainable Housing for Urban Poor Sector Project in Tamil Nadu: Development of three Working Women Hostels (St. Thomas Mount, Hosur, and Thiruvanamalai) by Tamil Nadu Working Women's Hostels Corporation Limited (53067-004)</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr"/>
       <c r="F62" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1600803/information-gathering-and-confirmation-survey-on-ai-human-resource-development-and-ecosystem-formati", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606477/inclusive-resilient-and-sustainable-housing-for-urban-poor-sector-project-in-tamil-nadu-development", "Apply")</f>
         <v/>
       </c>
     </row>
@@ -1903,110 +1903,18 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>Information gathering and confirmation survey on AI human resource development and ecosystem formation for the global South (QCBS-lump sum type)</t>
         </is>
       </c>
       <c r="C63" s="1" t="inlineStr"/>
       <c r="D63" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E63" s="1" t="inlineStr"/>
       <c r="F63" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa", "Apply")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" ht="80" customHeight="1">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B64" s="1" t="inlineStr">
-        <is>
-          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (Suchitwa Mission (State PMU))</t>
-        </is>
-      </c>
-      <c r="C64" s="1" t="inlineStr"/>
-      <c r="D64" s="1" t="inlineStr">
-        <is>
-          <t>Governance, Climate</t>
-        </is>
-      </c>
-      <c r="E64" s="1" t="inlineStr"/>
-      <c r="F64" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/738375/india-south-asia-p168633-kerala-solid-waste-management-project-procurement-plan", "Apply")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" ht="80" customHeight="1">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B65" s="1" t="inlineStr">
-        <is>
-          <t>RFP - Proposal for Digital Learning Centres – School Program</t>
-        </is>
-      </c>
-      <c r="C65" s="1" t="inlineStr"/>
-      <c r="D65" s="1" t="inlineStr">
-        <is>
-          <t>Learning</t>
-        </is>
-      </c>
-      <c r="E65" s="1" t="inlineStr"/>
-      <c r="F65" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606272/rfp-proposal-for-digital-learning-centres-school-program", "Apply")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" ht="80" customHeight="1">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B66" s="1" t="inlineStr">
-        <is>
-          <t>P507066 - Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER) - Procurement Plan (MPOWER-SPMU-MBMA)</t>
-        </is>
-      </c>
-      <c r="C66" s="1" t="inlineStr"/>
-      <c r="D66" s="1" t="inlineStr">
-        <is>
-          <t>Safety, Climate</t>
-        </is>
-      </c>
-      <c r="E66" s="1" t="inlineStr"/>
-      <c r="F66" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1351308/p507066-mpower-procurement-plan-mpower-spmu-mbma", "Apply")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" ht="80" customHeight="1">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B67" s="1" t="inlineStr">
-        <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
-        </is>
-      </c>
-      <c r="C67" s="1" t="inlineStr"/>
-      <c r="D67" s="1" t="inlineStr">
-        <is>
-          <t>Governance</t>
-        </is>
-      </c>
-      <c r="E67" s="1" t="inlineStr"/>
-      <c r="F67" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces", "Apply")</f>
+        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1600803/information-gathering-and-confirmation-survey-on-ai-human-resource-development-and-ecosystem-formati", "Apply")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Mon Feb 16 13:14:34 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,9 +482,10 @@
           <t>02/19/2026, 04:59 AM</t>
         </is>
       </c>
-      <c r="F2" s="1">
-        <f>HYPERLINK("https://estm.fa.em2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/job/28371/?location=India&amp;locationId=300000000440677&amp;locationLevel=country&amp;mode=location", "Apply")</f>
-        <v/>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>https://estm.fa.em2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/job/28371/?location=India&amp;locationId=300000000440677&amp;locationLevel=country&amp;mode=location</t>
+        </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
@@ -684,7 +685,7 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
@@ -694,9 +695,10 @@
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
-      <c r="F10" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other", "Apply")</f>
-        <v/>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
+        </is>
       </c>
     </row>
     <row r="11" ht="80" customHeight="1">
@@ -707,19 +709,20 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
-      <c r="F11" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1609019/ausbau-erneuerbarer-energien-expansion-of-renewable-energies", "Apply")</f>
-        <v/>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+        </is>
       </c>
     </row>
     <row r="12" ht="80" customHeight="1">
@@ -730,19 +733,20 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
-      <c r="F12" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
-        <v/>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+        </is>
       </c>
     </row>
     <row r="13" ht="80" customHeight="1">
@@ -753,7 +757,7 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
@@ -763,9 +767,10 @@
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
-      <c r="F13" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
-        <v/>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+        </is>
       </c>
     </row>
     <row r="14" ht="80" customHeight="1">
@@ -776,7 +781,7 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
@@ -786,9 +791,10 @@
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
-      <c r="F14" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal", "Apply")</f>
-        <v/>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="80" customHeight="1">
@@ -799,19 +805,20 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
-      <c r="F15" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu", "Apply")</f>
-        <v/>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+        </is>
       </c>
     </row>
     <row r="16" ht="80" customHeight="1">
@@ -822,19 +829,20 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
-      <c r="F16" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec", "Apply")</f>
-        <v/>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+        </is>
       </c>
     </row>
     <row r="17" ht="80" customHeight="1">
@@ -845,19 +853,20 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
-      <c r="F17" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t", "Apply")</f>
-        <v/>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+        </is>
       </c>
     </row>
     <row r="18" ht="80" customHeight="1">
@@ -868,19 +877,20 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
-      <c r="F18" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes", "Apply")</f>
-        <v/>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+        </is>
       </c>
     </row>
     <row r="19" ht="80" customHeight="1">
@@ -891,19 +901,20 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
-      <c r="F19" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter", "Apply")</f>
-        <v/>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+        </is>
       </c>
     </row>
     <row r="20" ht="80" customHeight="1">
@@ -914,19 +925,20 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
-      <c r="F20" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r", "Apply")</f>
-        <v/>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+        </is>
       </c>
     </row>
     <row r="21" ht="80" customHeight="1">
@@ -937,19 +949,20 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
-      <c r="F21" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e", "Apply")</f>
-        <v/>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+        </is>
       </c>
     </row>
     <row r="22" ht="80" customHeight="1">
@@ -960,19 +973,20 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
-      <c r="F22" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1", "Apply")</f>
-        <v/>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+        </is>
       </c>
     </row>
     <row r="23" ht="80" customHeight="1">
@@ -983,19 +997,20 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
-      <c r="F23" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr", "Apply")</f>
-        <v/>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+        </is>
       </c>
     </row>
     <row r="24" ht="80" customHeight="1">
@@ -1006,19 +1021,20 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
-      <c r="F24" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan", "Apply")</f>
-        <v/>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+        </is>
       </c>
     </row>
     <row r="25" ht="80" customHeight="1">
@@ -1029,19 +1045,20 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
-      <c r="F25" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-", "Apply")</f>
-        <v/>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+        </is>
       </c>
     </row>
     <row r="26" ht="80" customHeight="1">
@@ -1052,19 +1069,20 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
-      <c r="F26" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure", "Apply")</f>
-        <v/>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609019/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+        </is>
       </c>
     </row>
     <row r="27" ht="80" customHeight="1">
@@ -1075,19 +1093,20 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
-      <c r="F27" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
-        <v/>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+        </is>
       </c>
     </row>
     <row r="28" ht="80" customHeight="1">
@@ -1098,19 +1117,20 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
-      <c r="F28" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
-        <v/>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
       </c>
     </row>
     <row r="29" ht="80" customHeight="1">
@@ -1121,19 +1141,20 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
-      <c r="F29" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001", "Apply")</f>
-        <v/>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
       </c>
     </row>
     <row r="30" ht="80" customHeight="1">
@@ -1144,19 +1165,20 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
+          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
-      <c r="F30" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm", "Apply")</f>
-        <v/>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
+        </is>
       </c>
     </row>
     <row r="31" ht="80" customHeight="1">
@@ -1167,19 +1189,20 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
-      <c r="F31" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo", "Apply")</f>
-        <v/>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
+        </is>
       </c>
     </row>
     <row r="32" ht="80" customHeight="1">
@@ -1190,19 +1213,20 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
+          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
-      <c r="F32" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in", "Apply")</f>
-        <v/>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
+        </is>
       </c>
     </row>
     <row r="33" ht="80" customHeight="1">
@@ -1213,19 +1237,20 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
+          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
-      <c r="F33" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564", "Apply")</f>
-        <v/>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
+        </is>
       </c>
     </row>
     <row r="34" ht="80" customHeight="1">
@@ -1236,19 +1261,20 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
+          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
-      <c r="F34" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons", "Apply")</f>
-        <v/>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
+        </is>
       </c>
     </row>
     <row r="35" ht="80" customHeight="1">
@@ -1259,19 +1285,20 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
-      <c r="F35" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s", "Apply")</f>
-        <v/>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
+        </is>
       </c>
     </row>
     <row r="36" ht="80" customHeight="1">
@@ -1282,7 +1309,7 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
+          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
@@ -1292,9 +1319,10 @@
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
-      <c r="F36" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc", "Apply")</f>
-        <v/>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
+        </is>
       </c>
     </row>
     <row r="37" ht="80" customHeight="1">
@@ -1305,19 +1333,20 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
+          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
-      <c r="F37" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h", "Apply")</f>
-        <v/>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
+        </is>
       </c>
     </row>
     <row r="38" ht="80" customHeight="1">
@@ -1328,19 +1357,20 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
+          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
-      <c r="F38" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian", "Apply")</f>
-        <v/>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
+        </is>
       </c>
     </row>
     <row r="39" ht="80" customHeight="1">
@@ -1351,19 +1381,20 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
+          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
-      <c r="F39" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi", "Apply")</f>
-        <v/>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan</t>
+        </is>
       </c>
     </row>
     <row r="40" ht="80" customHeight="1">
@@ -1374,19 +1405,20 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
+          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
-      <c r="F40" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin", "Apply")</f>
-        <v/>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-</t>
+        </is>
       </c>
     </row>
     <row r="41" ht="80" customHeight="1">
@@ -1397,19 +1429,20 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
+          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
-      <c r="F41" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan", "Apply")</f>
-        <v/>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure</t>
+        </is>
       </c>
     </row>
     <row r="42" ht="80" customHeight="1">
@@ -1420,7 +1453,7 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
@@ -1430,9 +1463,10 @@
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
-      <c r="F42" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
-        <v/>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+        </is>
       </c>
     </row>
     <row r="43" ht="80" customHeight="1">
@@ -1443,19 +1477,20 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
-      <c r="F43" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific", "Apply")</f>
-        <v/>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+        </is>
       </c>
     </row>
     <row r="44" ht="80" customHeight="1">
@@ -1466,19 +1501,20 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
-      <c r="F44" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act", "Apply")</f>
-        <v/>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001</t>
+        </is>
       </c>
     </row>
     <row r="45" ht="80" customHeight="1">
@@ -1489,19 +1525,20 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
+          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
-      <c r="F45" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings", "Apply")</f>
-        <v/>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm</t>
+        </is>
       </c>
     </row>
     <row r="46" ht="80" customHeight="1">
@@ -1512,19 +1549,20 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
-      <c r="F46" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee", "Apply")</f>
-        <v/>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+        </is>
       </c>
     </row>
     <row r="47" ht="80" customHeight="1">
@@ -1535,7 +1573,7 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
@@ -1545,9 +1583,10 @@
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
-      <c r="F47" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep", "Apply")</f>
-        <v/>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in</t>
+        </is>
       </c>
     </row>
     <row r="48" ht="80" customHeight="1">
@@ -1558,7 +1597,7 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
+          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
@@ -1568,9 +1607,10 @@
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
-      <c r="F48" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha", "Apply")</f>
-        <v/>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564</t>
+        </is>
       </c>
     </row>
     <row r="49" ht="80" customHeight="1">
@@ -1581,19 +1621,20 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
+          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
-      <c r="F49" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance", "Apply")</f>
-        <v/>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons</t>
+        </is>
       </c>
     </row>
     <row r="50" ht="80" customHeight="1">
@@ -1604,19 +1645,20 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
-      <c r="F50" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu", "Apply")</f>
-        <v/>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
+        </is>
       </c>
     </row>
     <row r="51" ht="80" customHeight="1">
@@ -1627,19 +1669,20 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
+          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
-      <c r="F51" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c", "Apply")</f>
-        <v/>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc</t>
+        </is>
       </c>
     </row>
     <row r="52" ht="80" customHeight="1">
@@ -1650,19 +1693,20 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
+          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
-      <c r="F52" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s", "Apply")</f>
-        <v/>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h</t>
+        </is>
       </c>
     </row>
     <row r="53" ht="80" customHeight="1">
@@ -1673,19 +1717,20 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
+          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
-      <c r="F53" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution", "Apply")</f>
-        <v/>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian</t>
+        </is>
       </c>
     </row>
     <row r="54" ht="80" customHeight="1">
@@ -1696,19 +1741,20 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
+          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
-      <c r="F54" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper", "Apply")</f>
-        <v/>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi</t>
+        </is>
       </c>
     </row>
     <row r="55" ht="80" customHeight="1">
@@ -1719,19 +1765,20 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including WTP of 6.0 MLD and STP of 3.5, 1.5 MLD, for Rangpo including O&amp;M for 5 years</t>
+          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
-      <c r="F55" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448434/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
-        <v/>
+      <c r="F55" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin</t>
+        </is>
       </c>
     </row>
     <row r="56" ht="80" customHeight="1">
@@ -1742,7 +1789,7 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works, including WTP 4.0, MLD and STP 1.5 MLD, for Pakyong including O&amp;M for 5 years</t>
+          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
@@ -1752,9 +1799,10 @@
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
-      <c r="F56" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448435/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
-        <v/>
+      <c r="F56" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan</t>
+        </is>
       </c>
     </row>
     <row r="57" ht="80" customHeight="1">
@@ -1765,19 +1813,20 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: Comprehensive Water Supply &amp; Sanitation Improvement Works including STP of 2.5 MLD, for Singtam including O&amp;M for 5 years</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr"/>
-      <c r="F57" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1448436/57230-001-sikkim-integrated-urban-development-project", "Apply")</f>
-        <v/>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+        </is>
       </c>
     </row>
     <row r="58" ht="80" customHeight="1">
@@ -1788,19 +1837,20 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Bongaigaon/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Bongaigaon Town in Assam</t>
+          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
-      <c r="F58" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1445726/57262-ind-assam-urban-sector-development-project", "Apply")</f>
-        <v/>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific</t>
+        </is>
       </c>
     </row>
     <row r="59" ht="80" customHeight="1">
@@ -1811,19 +1861,20 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Goalpara/01: Construction and Ten-Year Operation and Maintenance of Water Supply Scheme for Goalpara Town in Assam</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr"/>
-      <c r="F59" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1418982/57262-ind-assam-urban-sector-development-project", "Apply")</f>
-        <v/>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+        </is>
       </c>
     </row>
     <row r="60" ht="80" customHeight="1">
@@ -1834,7 +1885,7 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Barpeta/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Barpeta Town in Assam</t>
+          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
@@ -1844,9 +1895,10 @@
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr"/>
-      <c r="F60" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404713/57262-ind-assam-urban-sector-development-project", "Apply")</f>
-        <v/>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings</t>
+        </is>
       </c>
     </row>
     <row r="61" ht="80" customHeight="1">
@@ -1857,19 +1909,20 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>57262-IND: Assam Urban Sector Development Project: AUSDP/WS/Nalbari/01: Augmentation with Ten-Year Operation and Maintenance of Water Supply Scheme for Nalbari Town in Assam</t>
+          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
-      <c r="F61" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1404712/57262-ind-assam-urban-sector-development-project", "Apply")</f>
-        <v/>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee</t>
+        </is>
       </c>
     </row>
     <row r="62" ht="80" customHeight="1">
@@ -1880,19 +1933,20 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>Inclusive, Resilient, and Sustainable Housing for Urban Poor Sector Project in Tamil Nadu: Development of three Working Women Hostels (St. Thomas Mount, Hosur, and Thiruvanamalai) by Tamil Nadu Working Women's Hostels Corporation Limited (53067-004)</t>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr"/>
-      <c r="F62" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1606477/inclusive-resilient-and-sustainable-housing-for-urban-poor-sector-project-in-tamil-nadu-development", "Apply")</f>
-        <v/>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
+        </is>
       </c>
     </row>
     <row r="63" ht="80" customHeight="1">
@@ -1903,7 +1957,7 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>Information gathering and confirmation survey on AI human resource development and ecosystem formation for the global South (QCBS-lump sum type)</t>
+          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
         </is>
       </c>
       <c r="C63" s="1" t="inlineStr"/>
@@ -1913,9 +1967,154 @@
         </is>
       </c>
       <c r="E63" s="1" t="inlineStr"/>
-      <c r="F63" s="1">
-        <f>HYPERLINK("https://www.developmentaid.org/tenders/view/1600803/information-gathering-and-confirmation-survey-on-ai-human-resource-development-and-ecosystem-formati", "Apply")</f>
-        <v/>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="80" customHeight="1">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr"/>
+      <c r="D64" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E64" s="1" t="inlineStr"/>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="80" customHeight="1">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr"/>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Safety, Climate</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr"/>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="80" customHeight="1">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr"/>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr"/>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c</t>
+        </is>
+      </c>
+    </row>
+    <row r="67" ht="80" customHeight="1">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr"/>
+      <c r="D67" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E67" s="1" t="inlineStr"/>
+      <c r="F67" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="80" customHeight="1">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr"/>
+      <c r="D68" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E68" s="1" t="inlineStr"/>
+      <c r="F68" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution</t>
+        </is>
+      </c>
+    </row>
+    <row r="69" ht="80" customHeight="1">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr"/>
+      <c r="D69" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E69" s="1" t="inlineStr"/>
+      <c r="F69" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Mon Feb 16 13:27:30 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -510,9 +510,10 @@
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
-      <c r="F3" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/697", "Knowledge Officer, C40 Cities Finance Facility (CFF)")</f>
-        <v/>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/697</t>
+        </is>
       </c>
     </row>
     <row r="4" ht="80" customHeight="1">
@@ -537,9 +538,10 @@
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
-      <c r="F4" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/698", "Senior Manager, Data Systems, Regions and Partnerships")</f>
-        <v/>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/698</t>
+        </is>
       </c>
     </row>
     <row r="5" ht="80" customHeight="1">
@@ -564,9 +566,10 @@
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
-      <c r="F5" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/699", "Programme Officer, C40 Cities Finance Facility (CFF)")</f>
-        <v/>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/699</t>
+        </is>
       </c>
     </row>
     <row r="6" ht="80" customHeight="1">
@@ -591,9 +594,10 @@
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
-      <c r="F6" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/700", "Operations Manager, GCoM")</f>
-        <v/>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/700</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="80" customHeight="1">
@@ -618,9 +622,10 @@
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
-      <c r="F7" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/701", "IT Helpdesk Technician (Paternity Cover)")</f>
-        <v/>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/701</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="80" customHeight="1">
@@ -645,9 +650,10 @@
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
-      <c r="F8" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/702", "Head of Regional Coordination, GCoM")</f>
-        <v/>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/702</t>
+        </is>
       </c>
     </row>
     <row r="9" ht="80" customHeight="1">
@@ -672,9 +678,10 @@
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
-      <c r="F9" s="1">
-        <f>HYPERLINK("https://c40.bamboohr.com/careers/703", "Manager, Adaptation Finance")</f>
-        <v/>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>https://c40.bamboohr.com/careers/703</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="80" customHeight="1">

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Tue Feb 17 04:15:23 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,23 +496,23 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Knowledge Officer, C40 Cities Finance Facility (CFF)</t>
+          <t>IT Helpdesk Technician (Paternity Cover)</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>Climate Finance, Knowledge and Partnerships - Belgium, Colombia, Denmark, Kenya, South Africa, &amp; UK (Hybrid)</t>
+          <t>Corporate Services - Copenhagen</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/697</t>
+          <t>https://c40.bamboohr.com/careers/701</t>
         </is>
       </c>
     </row>
@@ -524,23 +524,23 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Senior Manager, Data Systems, Regions and Partnerships</t>
+          <t>Head of Regional Coordination, GCoM</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>Global Covenant of Mayors - South Africa, United Kingdom</t>
+          <t>Global Covenant of Mayors - Brussels, London, Johannesburg, Rio de Janeiro</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/698</t>
+          <t>https://c40.bamboohr.com/careers/702</t>
         </is>
       </c>
     </row>
@@ -552,12 +552,12 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Programme Officer, C40 Cities Finance Facility (CFF)</t>
+          <t>Manager, Adaptation Finance</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Climate Finance, Knowledge and Partnerships - Belgium, Colombia, Denmark, Kenya, South Africa, &amp; UK (Hybrid)</t>
+          <t>Climate Finance, Knowledge and Partnerships - Kenya, South Africa</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -568,110 +568,94 @@
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/699</t>
+          <t>https://c40.bamboohr.com/careers/703</t>
         </is>
       </c>
     </row>
     <row r="6" ht="80" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Operations Manager, GCoM</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>Global Covenant of Mayors - Belgium, UK</t>
-        </is>
-      </c>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/700</t>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
         </is>
       </c>
     </row>
     <row r="7" ht="80" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>IT Helpdesk Technician (Paternity Cover)</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>Corporate Services - Copenhagen</t>
-        </is>
-      </c>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/701</t>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
         </is>
       </c>
     </row>
     <row r="8" ht="80" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Head of Regional Coordination, GCoM</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>Global Covenant of Mayors - Brussels, London, Johannesburg, Rio de Janeiro</t>
-        </is>
-      </c>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/702</t>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
         </is>
       </c>
     </row>
     <row r="9" ht="80" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Manager, Adaptation Finance</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>Climate Finance, Knowledge and Partnerships - Kenya, South Africa</t>
-        </is>
-      </c>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
           <t>Climate</t>
@@ -680,7 +664,7 @@
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/703</t>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -692,7 +676,7 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
@@ -704,7 +688,7 @@
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
         </is>
       </c>
     </row>
@@ -716,19 +700,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -740,19 +724,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
         </is>
       </c>
     </row>
@@ -764,19 +748,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
         </is>
       </c>
     </row>
@@ -788,19 +772,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
         </is>
       </c>
     </row>
@@ -812,19 +796,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
         </is>
       </c>
     </row>
@@ -836,19 +820,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -860,19 +844,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
         </is>
       </c>
     </row>
@@ -884,7 +868,7 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
@@ -896,7 +880,7 @@
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
         </is>
       </c>
     </row>
@@ -908,7 +892,7 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
@@ -920,7 +904,7 @@
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
         </is>
       </c>
     </row>
@@ -932,19 +916,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -956,19 +940,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
         </is>
       </c>
     </row>
@@ -980,19 +964,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1004,19 +988,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1028,19 +1012,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
         </is>
       </c>
     </row>
@@ -1052,19 +1036,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
         </is>
       </c>
     </row>
@@ -1076,19 +1060,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609019/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
         </is>
       </c>
     </row>
@@ -1100,19 +1084,19 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
         </is>
       </c>
     </row>
@@ -1124,19 +1108,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
         </is>
       </c>
     </row>
@@ -1148,19 +1132,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
         </is>
       </c>
     </row>
@@ -1172,19 +1156,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
+          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
         </is>
       </c>
     </row>
@@ -1196,19 +1180,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
+          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
         </is>
       </c>
     </row>
@@ -1220,19 +1204,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
+          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
         </is>
       </c>
     </row>
@@ -1244,19 +1228,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
+          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
         </is>
       </c>
     </row>
@@ -1268,19 +1252,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
+          <t>https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1292,19 +1276,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
+          <t>https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1300,7 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
@@ -1328,7 +1312,7 @@
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
+          <t>https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure</t>
         </is>
       </c>
     </row>
@@ -1340,19 +1324,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1364,19 +1348,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
+          <t>https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1388,19 +1372,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
+          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001</t>
         </is>
       </c>
     </row>
@@ -1412,19 +1396,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
+          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-</t>
+          <t>https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm</t>
         </is>
       </c>
     </row>
@@ -1436,19 +1420,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure</t>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
         </is>
       </c>
     </row>
@@ -1460,19 +1444,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in</t>
         </is>
       </c>
     </row>
@@ -1484,19 +1468,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
+          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564</t>
         </is>
       </c>
     </row>
@@ -1508,19 +1492,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
+          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001</t>
+          <t>https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons</t>
         </is>
       </c>
     </row>
@@ -1532,19 +1516,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm</t>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>
@@ -1556,19 +1540,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc</t>
         </is>
       </c>
     </row>
@@ -1580,19 +1564,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
+          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in</t>
+          <t>https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h</t>
         </is>
       </c>
     </row>
@@ -1604,19 +1588,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
+          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564</t>
+          <t>https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian</t>
         </is>
       </c>
     </row>
@@ -1628,19 +1612,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
+          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons</t>
+          <t>https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi</t>
         </is>
       </c>
     </row>
@@ -1652,7 +1636,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
@@ -1664,7 +1648,7 @@
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin</t>
         </is>
       </c>
     </row>
@@ -1676,19 +1660,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
+          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc</t>
+          <t>https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1700,19 +1684,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h</t>
+          <t>https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1724,19 +1708,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
+          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian</t>
+          <t>https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific</t>
         </is>
       </c>
     </row>
@@ -1748,19 +1732,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi</t>
+          <t>https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
         </is>
       </c>
     </row>
@@ -1772,19 +1756,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
+          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin</t>
+          <t>https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings</t>
         </is>
       </c>
     </row>
@@ -1796,19 +1780,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
+          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee</t>
         </is>
       </c>
     </row>
@@ -1820,19 +1804,19 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
         </is>
       </c>
     </row>
@@ -1844,19 +1828,19 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
+          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific</t>
+          <t>https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha</t>
         </is>
       </c>
     </row>
@@ -1868,19 +1852,19 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1892,19 +1876,19 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
+          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety, Climate</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings</t>
+          <t>https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu</t>
         </is>
       </c>
     </row>
@@ -1916,19 +1900,19 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
+          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee</t>
+          <t>https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c</t>
         </is>
       </c>
     </row>
@@ -1940,19 +1924,19 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr"/>
       <c r="F62" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
+          <t>https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1964,19 +1948,19 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
+          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
         </is>
       </c>
       <c r="C63" s="1" t="inlineStr"/>
       <c r="D63" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E63" s="1" t="inlineStr"/>
       <c r="F63" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha</t>
+          <t>https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution</t>
         </is>
       </c>
     </row>
@@ -1988,137 +1972,17 @@
       </c>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
+          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
         </is>
       </c>
       <c r="C64" s="1" t="inlineStr"/>
       <c r="D64" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E64" s="1" t="inlineStr"/>
       <c r="F64" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance</t>
-        </is>
-      </c>
-    </row>
-    <row r="65" ht="80" customHeight="1">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B65" s="1" t="inlineStr">
-        <is>
-          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
-        </is>
-      </c>
-      <c r="C65" s="1" t="inlineStr"/>
-      <c r="D65" s="1" t="inlineStr">
-        <is>
-          <t>Safety, Climate</t>
-        </is>
-      </c>
-      <c r="E65" s="1" t="inlineStr"/>
-      <c r="F65" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu</t>
-        </is>
-      </c>
-    </row>
-    <row r="66" ht="80" customHeight="1">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B66" s="1" t="inlineStr">
-        <is>
-          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
-        </is>
-      </c>
-      <c r="C66" s="1" t="inlineStr"/>
-      <c r="D66" s="1" t="inlineStr">
-        <is>
-          <t>Climate</t>
-        </is>
-      </c>
-      <c r="E66" s="1" t="inlineStr"/>
-      <c r="F66" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c</t>
-        </is>
-      </c>
-    </row>
-    <row r="67" ht="80" customHeight="1">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B67" s="1" t="inlineStr">
-        <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
-        </is>
-      </c>
-      <c r="C67" s="1" t="inlineStr"/>
-      <c r="D67" s="1" t="inlineStr">
-        <is>
-          <t>Governance, Learning</t>
-        </is>
-      </c>
-      <c r="E67" s="1" t="inlineStr"/>
-      <c r="F67" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
-        </is>
-      </c>
-    </row>
-    <row r="68" ht="80" customHeight="1">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B68" s="1" t="inlineStr">
-        <is>
-          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
-        </is>
-      </c>
-      <c r="C68" s="1" t="inlineStr"/>
-      <c r="D68" s="1" t="inlineStr">
-        <is>
-          <t>Climate</t>
-        </is>
-      </c>
-      <c r="E68" s="1" t="inlineStr"/>
-      <c r="F68" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution</t>
-        </is>
-      </c>
-    </row>
-    <row r="69" ht="80" customHeight="1">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B69" s="1" t="inlineStr">
-        <is>
-          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
-        </is>
-      </c>
-      <c r="C69" s="1" t="inlineStr"/>
-      <c r="D69" s="1" t="inlineStr">
-        <is>
-          <t>Climate</t>
-        </is>
-      </c>
-      <c r="E69" s="1" t="inlineStr"/>
-      <c r="F69" s="1" t="inlineStr">
         <is>
           <t>https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper</t>
         </is>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Wed Feb 18 04:17:48 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,19 +580,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
         </is>
       </c>
     </row>
@@ -604,19 +604,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
         </is>
       </c>
     </row>
@@ -628,7 +628,7 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
@@ -640,7 +640,7 @@
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
@@ -664,7 +664,7 @@
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
@@ -688,7 +688,7 @@
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -700,19 +700,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -724,19 +724,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
         </is>
       </c>
     </row>
@@ -748,19 +748,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
         </is>
       </c>
     </row>
@@ -772,19 +772,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
         </is>
       </c>
     </row>
@@ -796,19 +796,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
         </is>
       </c>
     </row>
@@ -820,19 +820,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
         </is>
       </c>
     </row>
@@ -844,19 +844,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
         </is>
       </c>
     </row>
@@ -868,19 +868,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
         </is>
       </c>
     </row>
@@ -892,19 +892,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
         </is>
       </c>
     </row>
@@ -916,19 +916,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -940,19 +940,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
         </is>
       </c>
     </row>
@@ -964,19 +964,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -988,19 +988,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
         </is>
       </c>
     </row>
@@ -1012,19 +1012,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
         </is>
       </c>
     </row>
@@ -1036,19 +1036,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
         </is>
       </c>
     </row>
@@ -1060,19 +1060,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
@@ -1096,7 +1096,7 @@
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1108,19 +1108,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
         </is>
       </c>
     </row>
@@ -1132,19 +1132,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
@@ -1168,7 +1168,7 @@
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
@@ -1192,7 +1192,7 @@
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
+          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -1204,19 +1204,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
+          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
         </is>
       </c>
     </row>
@@ -1228,19 +1228,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
+          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1252,19 +1252,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1276,19 +1276,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
+          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-</t>
+          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
         </is>
       </c>
     </row>
@@ -1300,19 +1300,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
+          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure</t>
+          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
         </is>
       </c>
     </row>
@@ -1324,19 +1324,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
         </is>
       </c>
     </row>
@@ -1348,19 +1348,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
+          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
         </is>
       </c>
     </row>
@@ -1372,19 +1372,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
+          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001</t>
+          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
         </is>
       </c>
     </row>
@@ -1396,19 +1396,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
+          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm</t>
+          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
         </is>
       </c>
     </row>
@@ -1420,19 +1420,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
+          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
@@ -1456,7 +1456,7 @@
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in</t>
+          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
         </is>
       </c>
     </row>
@@ -1468,19 +1468,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
+          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564</t>
+          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
         </is>
       </c>
     </row>
@@ -1492,19 +1492,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
+          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons</t>
+          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
         </is>
       </c>
     </row>
@@ -1516,19 +1516,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>46166-003 - Supporting Human Capital Development in Meghalaya (Phase 2) Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1411799/46166-003-supporting-human-capital-development-in-meghalaya-phase-2-project-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1540,19 +1540,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
+          <t>Construction of Swiss Pavilion for AI Summit as per the design and space provided at Pragati Maidan, New Delhi</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc</t>
+          <t>https://www.developmentaid.org/tenders/view/1608266/construction-of-swiss-pavilion-for-ai-summit-as-per-the-design-and-space-provided-at-pragati-maidan-</t>
         </is>
       </c>
     </row>
@@ -1564,19 +1564,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
+          <t>P168310 - State of Maharashtra's Agribusiness and Rural Transformation Project - Procurement Plan (Project Coordination Management Unit (PCMU-SMART))</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h</t>
+          <t>https://www.developmentaid.org/tenders/view/435581/india-south-asia-p168310-state-of-maharashtras-agribusiness-and-rural-transformation-project-procure</t>
         </is>
       </c>
     </row>
@@ -1588,19 +1588,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1612,19 +1612,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Transport Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi</t>
+          <t>https://www.developmentaid.org/tenders/view/1607892/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1636,19 +1636,19 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
+          <t>TA-9950 REG: PF: Data Science Expert - PF: Data Scientist PF: Data Science Expert (54079-001)</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin</t>
+          <t>https://www.developmentaid.org/tenders/view/1607886/ta-9950-reg-pf-data-science-expert-pf-data-scientist-pf-data-science-expert-54079-001</t>
         </is>
       </c>
     </row>
@@ -1660,19 +1660,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
+          <t>LOAN-4623 IND: Assam Urban Sector Development Project - AUSDP/CS/COM Community Mobilization Consultant (CMC) (57262-001)</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607884/loan-4623-ind-assam-urban-sector-development-project-ausdpcscom-community-mobilization-consultant-cm</t>
         </is>
       </c>
     </row>
@@ -1684,19 +1684,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
+          <t>Hiring of Event Management Agency For organisation of Two Workshops for the ILO in February 2026 in Bangalore</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1608036/hiring-of-event-management-agency-for-organisation-of-two-workshops-for-the-ilo-in-february-2026-in</t>
         </is>
       </c>
     </row>
@@ -1708,19 +1708,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
+          <t>Punjab Outcomes-Acceleration In School Education Operation - P500564</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific</t>
+          <t>https://www.developmentaid.org/tenders/view/1335085/punjab-outcomes-acceleration-in-school-education-operation-p500564</t>
         </is>
       </c>
     </row>
@@ -1732,19 +1732,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Strengthening Coastal Resilience and the Economy Project: Consultancy Service for Supervision of Construction of Turtle, Dugong &amp; Mangrove and International Bird Conservation Centre under TN SHORE Project</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1607773/strengthening-coastal-resilience-and-the-economy-project-consultancy-service-for-supervision-of-cons</t>
         </is>
       </c>
     </row>
@@ -1756,19 +1756,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings</t>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>
@@ -1780,19 +1780,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
+          <t>Implementation and Operation of FLR Monitoring, Evaluation, and Reporting Frameworks for Forest Landscape Restoration (FLR)</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee</t>
+          <t>https://www.developmentaid.org/tenders/view/1531583/implementation-and-operation-of-flr-monitoring-evaluation-and-reporting-frameworks-for-forest-landsc</t>
         </is>
       </c>
     </row>
@@ -1804,19 +1804,19 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+          <t>81319406 - Engagement of Agency/Consortium for the 'Global Best Practices and Climate Risk Finance for Heatwave Management</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
+          <t>https://www.developmentaid.org/tenders/view/1534310/81319406-engagement-of-agencyconsortium-for-the-global-best-practices-and-climate-risk-finance-for-h</t>
         </is>
       </c>
     </row>
@@ -1828,19 +1828,19 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>P178418- Tripura Rural Economic Growth and Service Delivery Project- Procurement Plan  (Samagra Shiksha Abhiyan (Education))</t>
+          <t>Renewable Energy Policy Advisory Services and Capacity Development of Government Officials in Indian States</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1016520/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-samagra-shiksha</t>
+          <t>https://www.developmentaid.org/tenders/view/1528202/renewable-energy-policy-advisory-services-and-capacity-development-of-government-officials-in-indian</t>
         </is>
       </c>
     </row>
@@ -1852,19 +1852,19 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>37909-045 - Trade and Supply Chain Finance Capacity Development: Technical Assistance</t>
+          <t>Unterstützung für die Partnerschaft für Grüne und Nachhaltige Entwicklung / Support for the Partnership for Green and Sustainable Development</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1584610/37909-045-trade-and-supply-chain-finance-capacity-development-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1607814/unterstutzung-fur-die-partnerschaft-fur-grune-und-nachhaltige-entwicklung-support-for-the-partnershi</t>
         </is>
       </c>
     </row>
@@ -1876,19 +1876,19 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>Meghalaya Multisectoral Project for Adolescent Wellbeing, Empowerment and Resilience (MPOWER): GD-8/Procurement of Furniture and Electrical Items for Office Setup of SPMU under MPOWER, MBMA</t>
+          <t>RFP - River Health and Water Dependency Assessment Betwa River Basin</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607091/meghalaya-multisectoral-project-for-adolescent-wellbeing-empowerment-and-resilience-mpower-gd-8procu</t>
+          <t>https://www.developmentaid.org/tenders/view/1607571/rfp-river-health-and-water-dependency-assessment-betwa-river-basin</t>
         </is>
       </c>
     </row>
@@ -1900,19 +1900,19 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>P154990- Jhelum and Tawi Flood Recovery Project - Procurement Plan (Jammu and Kashmir Medical Supplies Corporation Limited)</t>
+          <t>P172213 - Nagaland: Enhancing Classroom Teaching and Resources - Procurement Plan (Department of School Education (DSE))</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/577045/india-south-asia-p154990-jhelum-and-tawi-flood-recovery-project-jammu-and-kashmir-medical-supplies-c</t>
+          <t>https://www.developmentaid.org/tenders/view/539175/india-south-asia-p172213-nagaland-enhancing-classroom-teaching-and-resources-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Team Leader and Agri Expert (55154-002)</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat Rice and Millets under Public Distribution System - Logistics Sector Expert (55154-002)</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
@@ -1936,7 +1936,7 @@
       <c r="E62" s="1" t="inlineStr"/>
       <c r="F62" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606567/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1607502/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1948,19 +1948,19 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>RFP - Supply, Installation, Testing, Commissioning and Comprehensive Maintenance of Solar Energy Solutions: Grid Connected Rooftop Solar</t>
+          <t>Final evaluation of the Market Development Facility Phase 2 (Asia Pacific)</t>
         </is>
       </c>
       <c r="C63" s="1" t="inlineStr"/>
       <c r="D63" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E63" s="1" t="inlineStr"/>
       <c r="F63" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606912/rfp-supply-installation-testing-commissioning-and-comprehensive-maintenance-of-solar-energy-solution</t>
+          <t>https://www.developmentaid.org/tenders/view/1583551/final-evaluation-of-the-market-development-facility-phase-2-asia-pacific</t>
         </is>
       </c>
     </row>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>TA-9970 IND: Maharashtra Rural High Voltage Distribution System Expansion Program - Social Sector Expert Social Sector Expert (Green Livelihoods Expert) (50193-003)</t>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
         </is>
       </c>
       <c r="C64" s="1" t="inlineStr"/>
@@ -1984,7 +1984,79 @@
       <c r="E64" s="1" t="inlineStr"/>
       <c r="F64" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606542/ta-9970-ind-maharashtra-rural-high-voltage-distribution-system-expansion-program-social-sector-exper</t>
+          <t>https://www.developmentaid.org/tenders/view/1607171/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="80" customHeight="1">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Audio Quality Annotation of Student Voice Recordings</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr"/>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr"/>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607022/rfp-audio-quality-annotation-of-student-voice-recordings</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="80" customHeight="1">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>UNICEF Chhattisgarh is seeking manufacturers for the development and production of an innovative feeding tool (Complementary feeding bowl with spoon) to improve the diets of young children in CG</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr"/>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning, Safety</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr"/>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1607202/unicef-chhattisgarh-is-seeking-manufacturers-for-the-development-and-production-of-an-innovative-fee</t>
+        </is>
+      </c>
+    </row>
+    <row r="67" ht="80" customHeight="1">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr"/>
+      <c r="D67" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E67" s="1" t="inlineStr"/>
+      <c r="F67" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Fri Feb 20 04:12:08 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,108 +467,1444 @@
     <row r="2" ht="80" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>ESTM</t>
+          <t>C40</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Specialist – Operations, Fund Risk Management and Oversight (Open to all applicants)</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr"/>
-      <c r="D2" s="1" t="inlineStr"/>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>02/19/2026, 04:59 AM</t>
-        </is>
-      </c>
+          <t>Manager, Adaptation Finance</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Climate Finance, Knowledge and Partnerships - Kenya, South Africa</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>https://estm.fa.em2.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/job/28371/?location=India&amp;locationId=300000000440677&amp;locationLevel=country&amp;mode=location</t>
+          <t>https://c40.bamboohr.com/careers/703</t>
         </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>IT Helpdesk Technician (Paternity Cover)</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>Corporate Services - Copenhagen</t>
-        </is>
-      </c>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr"/>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/701</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
         </is>
       </c>
     </row>
     <row r="4" ht="80" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Head of Regional Coordination, GCoM</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Global Covenant of Mayors - Brussels, London, Johannesburg, Rio de Janeiro</t>
-        </is>
-      </c>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/702</t>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
         </is>
       </c>
     </row>
     <row r="5" ht="80" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Manager, Adaptation Finance</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>Climate Finance, Knowledge and Partnerships - Kenya, South Africa</t>
-        </is>
-      </c>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/703</t>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>GEF SAGF IV: Growth Equity Fund</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr"/>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr"/>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr"/>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr"/>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="80" customHeight="1">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr"/>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr"/>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="80" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr"/>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Safety</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr"/>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="80" customHeight="1">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr"/>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="80" customHeight="1">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr"/>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr"/>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="80" customHeight="1">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr"/>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr"/>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="80" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr"/>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="80" customHeight="1">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr"/>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="80" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr"/>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr"/>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="80" customHeight="1">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr"/>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="80" customHeight="1">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr"/>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="inlineStr"/>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="80" customHeight="1">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr"/>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr"/>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="80" customHeight="1">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr"/>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="inlineStr"/>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="80" customHeight="1">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr"/>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr"/>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="80" customHeight="1">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr"/>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr"/>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="80" customHeight="1">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr"/>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr"/>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="80" customHeight="1">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr"/>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning, Safety</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr"/>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="80" customHeight="1">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr"/>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Safety, Climate</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr"/>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="80" customHeight="1">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr"/>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr"/>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="80" customHeight="1">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr"/>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr"/>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="80" customHeight="1">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr"/>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr"/>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="80" customHeight="1">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr"/>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr"/>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="80" customHeight="1">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr"/>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr"/>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="80" customHeight="1">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr"/>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr"/>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="80" customHeight="1">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr"/>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr"/>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="80" customHeight="1">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr"/>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr"/>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="80" customHeight="1">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr"/>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr"/>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="80" customHeight="1">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr"/>
+      <c r="D34" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr"/>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="80" customHeight="1">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr"/>
+      <c r="D35" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr"/>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="80" customHeight="1">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr"/>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="inlineStr"/>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="80" customHeight="1">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr"/>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr"/>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="80" customHeight="1">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr"/>
+      <c r="D38" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr"/>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="80" customHeight="1">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr"/>
+      <c r="D39" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr"/>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="80" customHeight="1">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr"/>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr"/>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="80" customHeight="1">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr"/>
+      <c r="D41" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr"/>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="80" customHeight="1">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr"/>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E42" s="1" t="inlineStr"/>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="80" customHeight="1">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr"/>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr"/>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="80" customHeight="1">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr"/>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr"/>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="80" customHeight="1">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr"/>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Safety</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr"/>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="80" customHeight="1">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr"/>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr"/>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="80" customHeight="1">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr"/>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr"/>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="80" customHeight="1">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr"/>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr"/>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="80" customHeight="1">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr"/>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr"/>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="80" customHeight="1">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr"/>
+      <c r="D50" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr"/>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="80" customHeight="1">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr"/>
+      <c r="D51" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr"/>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="80" customHeight="1">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr"/>
+      <c r="D52" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E52" s="1" t="inlineStr"/>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="80" customHeight="1">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr"/>
+      <c r="D53" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr"/>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="80" customHeight="1">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr"/>
+      <c r="D54" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning, Safety</t>
+        </is>
+      </c>
+      <c r="E54" s="1" t="inlineStr"/>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="80" customHeight="1">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr"/>
+      <c r="D55" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr"/>
+      <c r="F55" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="80" customHeight="1">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr"/>
+      <c r="D56" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr"/>
+      <c r="F56" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="80" customHeight="1">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr"/>
+      <c r="D57" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr"/>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="80" customHeight="1">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr"/>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr"/>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="80" customHeight="1">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr"/>
+      <c r="D59" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr"/>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="80" customHeight="1">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr"/>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr"/>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" ht="80" customHeight="1">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr"/>
+      <c r="D61" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E61" s="1" t="inlineStr"/>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Sat Feb 21 04:03:06 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,24 +495,28 @@
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>DevelopmentAid</t>
+          <t>C40</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr"/>
+          <t>Media and Communications Senior Manager, GCoM</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Global Covenant of Mayors - Brazil, South Africa</t>
+        </is>
+      </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://c40.bamboohr.com/careers/705</t>
         </is>
       </c>
     </row>
@@ -524,19 +528,19 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
         </is>
       </c>
     </row>
@@ -548,19 +552,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
         </is>
       </c>
     </row>
@@ -572,19 +576,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>GEF SAGF IV: Growth Equity Fund</t>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
         </is>
       </c>
     </row>
@@ -596,19 +600,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
         </is>
       </c>
     </row>
@@ -620,19 +624,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
         </is>
       </c>
     </row>
@@ -644,19 +648,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -668,19 +672,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>
@@ -692,7 +696,7 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
@@ -704,7 +708,7 @@
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -716,19 +720,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
         </is>
       </c>
     </row>
@@ -740,19 +744,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
         </is>
       </c>
     </row>
@@ -764,19 +768,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
         </is>
       </c>
     </row>
@@ -788,19 +792,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
         </is>
       </c>
     </row>
@@ -812,19 +816,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -836,19 +840,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
         </is>
       </c>
     </row>
@@ -860,19 +864,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
         </is>
       </c>
     </row>
@@ -884,19 +888,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
+          <t>GEF SAGF IV: Growth Equity Fund</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
         </is>
       </c>
     </row>
@@ -908,19 +912,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
+          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
         </is>
       </c>
     </row>
@@ -932,19 +936,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
+          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
+          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
         </is>
       </c>
     </row>
@@ -956,19 +960,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
         </is>
       </c>
     </row>
@@ -980,19 +984,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
+          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
+          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
         </is>
       </c>
     </row>
@@ -1004,19 +1008,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
+          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1032,7 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
+          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
@@ -1040,7 +1044,7 @@
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
+          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
         </is>
       </c>
     </row>
@@ -1052,19 +1056,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
         </is>
       </c>
     </row>
@@ -1076,19 +1080,19 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1104,7 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
@@ -1112,7 +1116,7 @@
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1124,19 +1128,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
         </is>
       </c>
     </row>
@@ -1148,19 +1152,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
         </is>
       </c>
     </row>
@@ -1172,19 +1176,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1196,19 +1200,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
+          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1220,19 +1224,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1244,19 +1248,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
         </is>
       </c>
     </row>
@@ -1268,19 +1272,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
         </is>
       </c>
     </row>
@@ -1292,19 +1296,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
         </is>
       </c>
     </row>
@@ -1316,19 +1320,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
         </is>
       </c>
     </row>
@@ -1340,19 +1344,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
         </is>
       </c>
     </row>
@@ -1364,19 +1368,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1388,19 +1392,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -1412,19 +1416,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1436,19 +1440,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
         </is>
       </c>
     </row>
@@ -1460,19 +1464,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
         </is>
       </c>
     </row>
@@ -1484,19 +1488,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
         </is>
       </c>
     </row>
@@ -1508,19 +1512,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
         </is>
       </c>
     </row>
@@ -1532,19 +1536,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
+          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
         </is>
       </c>
     </row>
@@ -1556,19 +1560,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
         </is>
       </c>
     </row>
@@ -1580,7 +1584,7 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
@@ -1592,7 +1596,7 @@
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
         </is>
       </c>
     </row>
@@ -1604,7 +1608,7 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
@@ -1616,7 +1620,7 @@
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1632,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing dry stone check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
@@ -1640,7 +1644,7 @@
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608977/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1652,19 +1656,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing crate wire check barriers in project GP,s of Sirmour Distt.</t>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1579382/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
         </is>
       </c>
     </row>
@@ -1676,19 +1680,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>TA-9849 IND: TA 9849-IND: India Urban and Water Projects Support Facility (53067-002) - Environment Safeguards Expert (53067-002)</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608441/ta-9849-ind-ta-9849-ind-india-urban-and-water-projects-support-facility-53067-002-environment-safegu</t>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -1700,7 +1704,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>TA-10721 IND: Support for Development of Sustainable Metro Rail Projects for Nagpur Metro Rail Project (Phase 2) - B/CS-1 Consulting services to design and develop a large battery storage system of 8 MW per day capacity and undertake technology demonstration pilot projects at two locations with 15 years of operation and (59279-001)</t>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
@@ -1712,7 +1716,7 @@
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608429/ta-10721-ind-support-for-development-of-sustainable-metro-rail-projects-for-nagpur-metro-rail-projec</t>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
         </is>
       </c>
     </row>
@@ -1724,19 +1728,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>81322849 - Capacity development and organisational support for convergent implementation of measures to improve water security in rural India</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1593414/81322849-capacity-development-and-organisational-support-for-convergent-implementation-of-measures-t</t>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
         </is>
       </c>
     </row>
@@ -1748,19 +1752,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>Consulting, Feasibility Study (Climate Resilience and Ecosystem Services in Forest Landscapes)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608627/consulting-feasibility-study-climate-resilience-and-ecosystem-services-in-forest-landscapes</t>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
         </is>
       </c>
     </row>
@@ -1772,19 +1776,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4322 IND: Enhancing Connectivity and Sustainability in Bihar Roads Project - 1 Expression of Interest for procurement of services for survey, data collection, design, development, implementation, operation and maintenance of road asset management system (54364-001)</t>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605060/loan-4322-ind-enhancing-connectivity-and-sustainability-in-bihar-roads-project-1-expression-of-inter</t>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1800,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>TA-10469 IND: Knowledge and Capacity Building for Catalyzing Green Growth and Strengthening Climate Resilience - Climate Risk Assessment and Bamboo Resource Mapping for Climate Strategies and Agriculture Investment Planning in Maharashtra, India (58389-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
@@ -1808,7 +1812,7 @@
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1603067/ta-10469-ind-knowledge-and-capacity-building-for-catalyzing-green-growth-and-strengthening-climate-r</t>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1820,19 +1824,19 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>Support in the Implementation of Basin Management Measures and District Ganga Plans</t>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1550511/support-in-the-implementation-of-basin-management-measures-and-district-ganga-plans</t>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
         </is>
       </c>
     </row>
@@ -1844,19 +1848,19 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>Expression of Interest for Selection of Business Associate(s) / Partner(s)/ JV / Consortium / partnership, for exploring Consulting / OEM assignments in Middle East, Africa, Europe, India and Southeast Asian Countries.</t>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608411/expression-of-interest-for-selection-of-business-associates-partners-jv-consortium-partnership-for-e</t>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
         </is>
       </c>
     </row>
@@ -1868,7 +1872,7 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>43253-025 - Karnataka Integrated Urban Water Management Investment Program - Tranche 1</t>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
@@ -1880,7 +1884,7 @@
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608368/43253-025-karnataka-integrated-urban-water-management-investment-program-tranche-1</t>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1896,7 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>Punjab Municipal Services Improvement Project: Direct RFP for hiring of Agency for Communication, Outreach, Digital Media Management &amp; Stakeholders Engagement in Municipal Corporation Amritsar and Ludhiana under PMSIP</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
@@ -1904,7 +1908,31 @@
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1606067/punjab-municipal-services-improvement-project-direct-rfp-for-hiring-of-agency-for-communication-outr</t>
+          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="80" customHeight="1">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr"/>
+      <c r="D62" s="1" t="inlineStr">
+        <is>
+          <t>Climate</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr"/>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Tue Feb 24 04:14:55 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,51 +472,47 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Manager, Adaptation Finance</t>
+          <t>Media and Communications Senior Manager, GCoM</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Climate Finance, Knowledge and Partnerships - Kenya, South Africa</t>
+          <t>Global Covenant of Mayors - Brazil, South Africa</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/703</t>
+          <t>https://c40.bamboohr.com/careers/705</t>
         </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>DevelopmentAid</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Media and Communications Senior Manager, GCoM</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>Global Covenant of Mayors - Brazil, South Africa</t>
-        </is>
-      </c>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr"/>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/705</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -528,19 +524,19 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Printing of Collaterals’ for State Refresher Training</t>
+          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
         </is>
       </c>
     </row>
@@ -552,19 +548,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
         </is>
       </c>
     </row>
@@ -576,19 +572,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
         </is>
       </c>
     </row>
@@ -600,19 +596,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
         </is>
       </c>
     </row>
@@ -624,19 +620,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
         </is>
       </c>
     </row>
@@ -648,19 +644,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
         </is>
       </c>
     </row>
@@ -672,19 +668,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
         </is>
       </c>
     </row>
@@ -696,19 +692,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
         </is>
       </c>
     </row>
@@ -720,19 +716,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -744,19 +740,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>
@@ -768,19 +764,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -792,19 +788,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
+          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
+          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
         </is>
       </c>
     </row>
@@ -816,19 +812,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
+          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
         </is>
       </c>
     </row>
@@ -840,19 +836,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
         </is>
       </c>
     </row>
@@ -864,19 +860,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
         </is>
       </c>
     </row>
@@ -888,19 +884,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>GEF SAGF IV: Growth Equity Fund</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -912,19 +908,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
         </is>
       </c>
     </row>
@@ -936,19 +932,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
         </is>
       </c>
     </row>
@@ -960,19 +956,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+          <t>GEF SAGF IV: Growth Equity Fund</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
         </is>
       </c>
     </row>
@@ -984,19 +980,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
         </is>
       </c>
     </row>
@@ -1008,19 +1004,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
         </is>
       </c>
     </row>
@@ -1032,19 +1028,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
         </is>
       </c>
     </row>
@@ -1056,19 +1052,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
         </is>
       </c>
     </row>
@@ -1080,19 +1076,19 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1100,7 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
@@ -1116,7 +1112,7 @@
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1124,7 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
@@ -1140,7 +1136,7 @@
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1148,7 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
@@ -1164,7 +1160,7 @@
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
+          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1172,7 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
@@ -1188,7 +1184,7 @@
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1200,19 +1196,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
         </is>
       </c>
     </row>
@@ -1224,19 +1220,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
         </is>
       </c>
     </row>
@@ -1248,19 +1244,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
+          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1268,7 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
@@ -1284,7 +1280,7 @@
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1296,19 +1292,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
+          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1320,19 +1316,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
+          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
+          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1340,7 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
@@ -1356,7 +1352,7 @@
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
         </is>
       </c>
     </row>
@@ -1368,19 +1364,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
+          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
         </is>
       </c>
     </row>
@@ -1392,19 +1388,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1412,7 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
@@ -1428,7 +1424,7 @@
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
         </is>
       </c>
     </row>
@@ -1440,19 +1436,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
+          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1464,7 +1460,7 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
@@ -1476,7 +1472,7 @@
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -1488,19 +1484,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1512,19 +1508,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
+          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
+          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
         </is>
       </c>
     </row>
@@ -1536,19 +1532,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
+          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
         </is>
       </c>
     </row>
@@ -1560,19 +1556,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
         </is>
       </c>
     </row>
@@ -1584,19 +1580,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
         </is>
       </c>
     </row>
@@ -1608,19 +1604,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
         </is>
       </c>
     </row>
@@ -1632,19 +1628,19 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1652,7 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
@@ -1668,7 +1664,7 @@
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
         </is>
       </c>
     </row>
@@ -1680,19 +1676,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
         </is>
       </c>
     </row>
@@ -1704,19 +1700,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1728,19 +1724,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
         </is>
       </c>
     </row>
@@ -1752,7 +1748,7 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
@@ -1764,7 +1760,7 @@
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1772,7 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
@@ -1788,7 +1784,7 @@
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
         </is>
       </c>
     </row>
@@ -1800,19 +1796,19 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
         </is>
       </c>
     </row>
@@ -1824,19 +1820,19 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
+          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1844,7 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
+          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
@@ -1860,7 +1856,7 @@
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
         </is>
       </c>
     </row>
@@ -1872,19 +1868,19 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1896,19 +1892,19 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Young Professional-II (04) (Project Data Management) (57041-001)</t>
+          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602444/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
         </is>
       </c>
     </row>
@@ -1920,19 +1916,43 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>Integrated Urban Climate Action for Low-Carbon &amp; Resilient Cities (Urban-Act)</t>
+          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
       <c r="D62" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr"/>
       <c r="F62" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1608947/integrated-urban-climate-action-for-low-carbon-resilient-cities-urban-act</t>
+          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" ht="80" customHeight="1">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr"/>
+      <c r="D63" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E63" s="1" t="inlineStr"/>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Wed Feb 25 04:16:55 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,47 +472,51 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Media and Communications Senior Manager, GCoM</t>
+          <t>Senior Manager, Data System Development</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Global Covenant of Mayors - Brazil, South Africa</t>
+          <t>Business Planning, Measurement and Innovation - Brazil, Colombia, Denmark, US, UK</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>https://c40.bamboohr.com/careers/705</t>
+          <t>https://c40.bamboohr.com/careers/704</t>
         </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>DevelopmentAid</t>
+          <t>C40</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr"/>
+          <t>Media and Communications Senior Manager, GCoM</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Global Covenant of Mayors - Brazil, South Africa</t>
+        </is>
+      </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://c40.bamboohr.com/careers/705</t>
         </is>
       </c>
     </row>
@@ -524,7 +528,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
@@ -536,7 +540,7 @@
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -548,19 +552,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
+          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
+          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
         </is>
       </c>
     </row>
@@ -572,7 +576,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
+          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
@@ -584,7 +588,7 @@
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
+          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
         </is>
       </c>
     </row>
@@ -596,19 +600,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Printing of Collaterals’ for State Refresher Training</t>
+          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -620,19 +624,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
         </is>
       </c>
     </row>
@@ -644,19 +648,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
         </is>
       </c>
     </row>
@@ -668,19 +672,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
         </is>
       </c>
     </row>
@@ -692,19 +696,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -716,19 +720,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
+          <t>Evidence for AI in Health (EVAH)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
+          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
         </is>
       </c>
     </row>
@@ -740,19 +744,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -764,19 +768,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
+          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
+          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -788,19 +792,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
+          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
+          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
         </is>
       </c>
     </row>
@@ -812,19 +816,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
+          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
+          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
         </is>
       </c>
     </row>
@@ -836,19 +840,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -860,19 +864,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -884,19 +888,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
+          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
+          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
         </is>
       </c>
     </row>
@@ -908,7 +912,7 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
@@ -920,7 +924,7 @@
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
         </is>
       </c>
     </row>
@@ -932,19 +936,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
         </is>
       </c>
     </row>
@@ -956,19 +960,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>GEF SAGF IV: Growth Equity Fund</t>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
         </is>
       </c>
     </row>
@@ -980,19 +984,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
         </is>
       </c>
     </row>
@@ -1004,19 +1008,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
         </is>
       </c>
     </row>
@@ -1028,19 +1032,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
         </is>
       </c>
     </row>
@@ -1052,19 +1056,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
         </is>
       </c>
     </row>
@@ -1076,19 +1080,19 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -1100,19 +1104,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1128,7 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
@@ -1136,7 +1140,7 @@
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
         </is>
       </c>
     </row>
@@ -1148,19 +1152,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
         </is>
       </c>
     </row>
@@ -1172,19 +1176,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
         </is>
       </c>
     </row>
@@ -1196,19 +1200,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
         </is>
       </c>
     </row>
@@ -1220,19 +1224,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
         </is>
       </c>
     </row>
@@ -1244,19 +1248,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
         </is>
       </c>
     </row>
@@ -1268,19 +1272,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
+          <t>GEF SAGF IV: Growth Equity Fund</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
         </is>
       </c>
     </row>
@@ -1292,19 +1296,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
+          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
         </is>
       </c>
     </row>
@@ -1316,19 +1320,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
+          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
+          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
         </is>
       </c>
     </row>
@@ -1340,19 +1344,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
         </is>
       </c>
     </row>
@@ -1364,19 +1368,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
+          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
+          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
         </is>
       </c>
     </row>
@@ -1388,19 +1392,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
+          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1412,7 +1416,7 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
+          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
@@ -1424,7 +1428,7 @@
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
+          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
         </is>
       </c>
     </row>
@@ -1436,19 +1440,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
         </is>
       </c>
     </row>
@@ -1460,19 +1464,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
         </is>
       </c>
     </row>
@@ -1484,7 +1488,7 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
@@ -1496,7 +1500,7 @@
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1508,19 +1512,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
         </is>
       </c>
     </row>
@@ -1532,19 +1536,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
+          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
         </is>
       </c>
     </row>
@@ -1556,19 +1560,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1580,19 +1584,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
+          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1604,19 +1608,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1628,19 +1632,19 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>EoI - For Empanelment of agencies for Impact Assessment / Evaluation Services under Programmes for Development and Impact</t>
+          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609663/eoi-for-empanelment-of-agencies-for-impact-assessment-evaluation-services-under-programmes-for-devel</t>
+          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
         </is>
       </c>
     </row>
@@ -1652,19 +1656,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>RFP - Early-Stage Impact Assessment-CDRI SWP 23-26</t>
+          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609606/rfp-early-stage-impact-assessment-cdri-swp-23-26</t>
+          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
         </is>
       </c>
     </row>
@@ -1676,19 +1680,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>Mirova Energy Transition Emerging Asia (METEA)</t>
+          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609692/mirova-energy-transition-emerging-asia-metea</t>
+          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
         </is>
       </c>
     </row>
@@ -1700,19 +1704,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609597/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
         </is>
       </c>
     </row>
@@ -1724,19 +1728,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Hiring consultancy firm for filing GST, VAT, IGST Refund Claims and related tasks for the ILO New Delhi office</t>
+          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609700/hiring-consultancy-firm-for-filing-gst-vat-igst-refund-claims-and-related-tasks-for-the-ilo-new-delh</t>
+          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
         </is>
       </c>
     </row>
@@ -1748,19 +1752,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4411 IND: Building India's Clean Plant Program - IARI-staff-C S09 IARI staff - virologists and other staff - Lab Assistant (02) (Plant Material Management) (57041-001)</t>
+          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1602442/loan-4411-ind-building-indias-clean-plant-program-iari-staff-c-s09-iari-staff-virologists-and-other</t>
+          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1772,19 +1776,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4291 IND: Himachal Pradesh Subtropical Horticulture, Irrigation, and Value Addition Project - CS 10 Communications and digital contents for Information Education and Knowledge Management under HPSHIVA Project (53189-002)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609118/loan-4291-ind-himachal-pradesh-subtropical-horticulture-irrigation-and-value-addition-project-cs-10</t>
+          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1796,19 +1800,19 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Knowledge and Learning Specialist (National) (58369-001)</t>
+          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
       <c r="D57" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609114/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-knowledge-and-learning-speci</t>
+          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
         </is>
       </c>
     </row>
@@ -1820,7 +1824,7 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Fecal Sludge Management and Urban Institutional Expert (National) (58369-001)</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
@@ -1832,7 +1836,7 @@
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1609113/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-fecal-sludge-management-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
         </is>
       </c>
     </row>
@@ -1844,19 +1848,19 @@
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>Request For Proposal For Hiring of Technical Partner Agency for Designing, Development and Implementation of AI-Enabled Learning and Knowledge Sharing Platform for ISA</t>
+          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr"/>
       <c r="D59" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr"/>
       <c r="F59" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589295/request-for-proposal-for-hiring-of-technical-partner-agency-for-designing-development-and-implementa</t>
+          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
         </is>
       </c>
     </row>
@@ -1868,19 +1872,19 @@
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB PGT PALAKKAD)</t>
+          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr"/>
       <c r="D60" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr"/>
       <c r="F60" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095526/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-palakkad-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
         </is>
       </c>
     </row>
@@ -1892,67 +1896,19 @@
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>P166020 - West Bengal Transport and Logistics Spatial Development Project - Procurement Plan (West Bengal Transport Infrastructure Development Corporation Limited)</t>
+          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr"/>
       <c r="D61" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr"/>
       <c r="F61" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/485630/india-south-asia-p166020-west-bengal-transport-and-logistics-spatial-development-project-procurement</t>
-        </is>
-      </c>
-    </row>
-    <row r="62" ht="80" customHeight="1">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B62" s="1" t="inlineStr">
-        <is>
-          <t>P179935- Enhancing Landscape and Ecosystem Management (ELEMENT) Project - Procurement Plan (State Forest Development Agency, Tripura)</t>
-        </is>
-      </c>
-      <c r="C62" s="1" t="inlineStr"/>
-      <c r="D62" s="1" t="inlineStr">
-        <is>
-          <t>Governance, Learning</t>
-        </is>
-      </c>
-      <c r="E62" s="1" t="inlineStr"/>
-      <c r="F62" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1161054/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-procurement-plan-engli</t>
-        </is>
-      </c>
-    </row>
-    <row r="63" ht="80" customHeight="1">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B63" s="1" t="inlineStr">
-        <is>
-          <t>Request for Proposals (RFP): Consulting Agency for Identifying High Growth Livelihoods and Market Access Challenges</t>
-        </is>
-      </c>
-      <c r="C63" s="1" t="inlineStr"/>
-      <c r="D63" s="1" t="inlineStr">
-        <is>
-          <t>Governance</t>
-        </is>
-      </c>
-      <c r="E63" s="1" t="inlineStr"/>
-      <c r="F63" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1598904/request-for-proposals-rfp-consulting-agency-for-identifying-high-growth-livelihoods-and-market-acces</t>
+          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Thu Feb 26 04:13:04 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,19 +528,19 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>Skills: National ITI Upgradation Program - P507910</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1425157/skills-national-iti-upgradation-program-p507910</t>
         </is>
       </c>
     </row>
@@ -552,19 +552,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: 04. SIUDP /DRY/THCC-01 - Design Build: Three Transit hubs cum community complex (THCCs) in Rangpo (Lot - 1), Ranipool (Lot - 2), and Pakyong (Lot - 3)</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
+          <t>https://www.developmentaid.org/tenders/view/1438614/57230-001-sikkim-integrated-urban-development-project</t>
         </is>
       </c>
     </row>
@@ -576,19 +576,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
+          <t>LOAN 57262-001 IND: Assam Urban Sector Development Project - AUSDP/CMS/01 Project Management and Supervision Consultants (PMSC)</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1266713/loan-57262-001-ind-assam-urban-sector-development-project-ausdpcms01-project-management-and-supervis</t>
         </is>
       </c>
     </row>
@@ -600,19 +600,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
+          <t>Hiring of an Agency for Development of an Operational &amp; Implementation Plan for Solar Global Capability Center (GCC)</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1614087/hiring-of-an-agency-for-development-of-an-operational-implementation-plan-for-solar-global-capabilit</t>
         </is>
       </c>
     </row>
@@ -624,19 +624,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
+          <t>TA-9844 IND: Supporting Education and Skills Development Facility - Financial Management Specialist (53277-001)</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
+          <t>https://www.developmentaid.org/tenders/view/1613681/ta-9844-ind-supporting-education-and-skills-development-facility-financial-management-specialist-532</t>
         </is>
       </c>
     </row>
@@ -648,19 +648,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
+          <t>RFP-011-IND-2026 - Agency for Development of a Gender-Responsive SDG framework</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
+          <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
         </is>
       </c>
     </row>
@@ -672,19 +672,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
+          <t>TA-10416 IND: Promoting Disaster Risk Insurance (54081-001)</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
+          <t>https://www.developmentaid.org/tenders/view/1613677/ta-10416-ind-promoting-disaster-risk-insurance-54081-001</t>
         </is>
       </c>
     </row>
@@ -696,19 +696,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>
@@ -720,19 +720,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Evidence for AI in Health (EVAH)</t>
+          <t>Carpl.AI, Inc</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
+          <t>https://www.developmentaid.org/tenders/view/1614052/carplai-inc</t>
         </is>
       </c>
     </row>
@@ -744,19 +744,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
+          <t>RFQ - Final Evaluation of the UNESCO-Guerlain Women for Bees project</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
+          <t>https://www.developmentaid.org/tenders/view/1614000/rfq-final-evaluation-of-the-unesco-guerlain-women-for-bees-project</t>
         </is>
       </c>
     </row>
@@ -768,19 +768,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
+          <t>TA-6742 REG: Building Coastal Resilience through Nature-Based and Integrated Solutions - Project Evaluation Specialist (54212-001)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1613663/ta-6742-reg-building-coastal-resilience-through-nature-based-and-integrated-solutions-project-evalua</t>
         </is>
       </c>
     </row>
@@ -792,19 +792,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -816,19 +816,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -840,19 +840,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
+          <t>LOAN-4166 IND: Assam Skill University Project - CS11 Project Management Support for Capacity Development of Assam Civil Service (53277-002)</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
+          <t>https://www.developmentaid.org/tenders/view/1599394/loan-4166-ind-assam-skill-university-project-cs11-project-management-support-for-capacity-developmen</t>
         </is>
       </c>
     </row>
@@ -864,19 +864,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
         </is>
       </c>
     </row>
@@ -888,19 +888,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
+          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
+          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
         </is>
       </c>
     </row>
@@ -912,19 +912,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
+          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
+          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -936,19 +936,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
+          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
+          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
         </is>
       </c>
     </row>
@@ -960,19 +960,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Printing of Collaterals’ for State Refresher Training</t>
+          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
         </is>
       </c>
     </row>
@@ -984,19 +984,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
         </is>
       </c>
     </row>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
@@ -1020,7 +1020,7 @@
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1032,19 +1032,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+          <t>Evidence for AI in Health (EVAH)</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
         </is>
       </c>
     </row>
@@ -1056,19 +1056,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
+          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
@@ -1092,7 +1092,7 @@
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
+          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1104,19 +1104,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
+          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
         </is>
       </c>
     </row>
@@ -1128,19 +1128,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
+          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
+          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
         </is>
       </c>
     </row>
@@ -1152,19 +1152,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -1176,19 +1176,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>SC 125823 IND: Karnataka Integrated Urban Water Management Investment Program - Tranche 2 - Financial Management Specialist</t>
+          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
@@ -1212,7 +1212,7 @@
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1589870/sc-125823-ind-karnataka-integrated-urban-water-management-investment-program-tranche-2</t>
+          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
@@ -1236,7 +1236,7 @@
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
         </is>
       </c>
     </row>
@@ -1248,19 +1248,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
         </is>
       </c>
     </row>
@@ -1272,19 +1272,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>GEF SAGF IV: Growth Equity Fund</t>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
         </is>
       </c>
     </row>
@@ -1296,19 +1296,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
         </is>
       </c>
     </row>
@@ -1320,19 +1320,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
         </is>
       </c>
     </row>
@@ -1344,19 +1344,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
         </is>
       </c>
     </row>
@@ -1368,19 +1368,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
         </is>
       </c>
     </row>
@@ -1392,19 +1392,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
         </is>
       </c>
     </row>
@@ -1440,19 +1440,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
         </is>
       </c>
     </row>
@@ -1464,19 +1464,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
         </is>
       </c>
     </row>
@@ -1488,19 +1488,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
         </is>
       </c>
     </row>
@@ -1512,19 +1512,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
         </is>
       </c>
     </row>
@@ -1536,19 +1536,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: PDKV AKOLA -Development of Crop Weather Calendars, Sowing Advisories and Spectral Response to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>GEF SAGF IV: Growth Equity Fund</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610858/maharashtra-project-on-climate-resilient-agriculture-phase-ii-pdkv-akola-development-of-crop-weather</t>
+          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
         </is>
       </c>
     </row>
@@ -1560,19 +1560,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Secondary water storage structure for gravity irrigation  Schemes in different G.P.'s under APO Unit Rajgarh of Sirmaur District</t>
+          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610840/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
         </is>
       </c>
     </row>
@@ -1584,19 +1584,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Drainage line treatment by constructing cement concrete check barriers in project GP,s of Sirmour Distt</t>
+          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610839/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
         </is>
       </c>
     </row>
@@ -1608,19 +1608,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Renovation of old ponds in Project GP's of Sirmour Distt</t>
+          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610836/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference (tor) for Developing a Visually Appealing Illustrated and Annotated Map Poster (based on Technical Data) Showing the Natural Assets of Delhi Under the Developing 75 Food Gardens in 4 Mega Cities in India Project</t>
+          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
@@ -1644,7 +1644,7 @@
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610798/terms-of-reference-tor-for-developing-a-visually-appealing-illustrated-and-annotated-map-poster-base</t>
+          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>TA-10488 REG: City Resilience, Affordable Housing, Sustainable Tourism, and Inclusive Economic Growth for Livable Cities - Structural Engineer (58349-002)</t>
+          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
@@ -1668,7 +1668,7 @@
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1605066/ta-10488-reg-city-resilience-affordable-housing-sustainable-tourism-and-inclusive-economic-growth-fo</t>
+          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
         </is>
       </c>
     </row>
@@ -1680,19 +1680,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>P179337- Assam State Secondary Healthcare Initiative for Service Delivery Transformation (ASSIST) Project - Procurement Plan (Assam Health Infrastructure Development and Management Society)</t>
+          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1080539/india-south-asia-p179337-assam-state-secondary-healthcare-initiative-for-service-delivery-transforma</t>
+          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
         </is>
       </c>
     </row>
@@ -1704,19 +1704,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>55252-001 - Maharashtra Sustainable Climate-Resilient Coastal Protection and Management Project: Procurement Plan</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1378025/55252-001-maharashtra-sustainable-climate-resilient-coastal-protection-and-management-project-procur</t>
+          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
         </is>
       </c>
     </row>
@@ -1728,19 +1728,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Solarenergie im ländlichen Raum Indiens / Solar energy in rural India</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610293/solarenergie-im-landlichen-raum-indiens-solar-energy-in-rural-india</t>
+          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
         </is>
       </c>
     </row>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>56300-002 - Madhya Pradesh Renewable Energy Implementation Support: Technical Assistance</t>
+          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
@@ -1764,7 +1764,7 @@
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610325/56300-002-madhya-pradesh-renewable-energy-implementation-support-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
         </is>
       </c>
     </row>
@@ -1776,139 +1776,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610299/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" ht="80" customHeight="1">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B57" s="1" t="inlineStr">
-        <is>
-          <t>Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project: Engagement of Project Management Consultant</t>
-        </is>
-      </c>
-      <c r="C57" s="1" t="inlineStr"/>
-      <c r="D57" s="1" t="inlineStr">
-        <is>
-          <t>Governance, Climate</t>
-        </is>
-      </c>
-      <c r="E57" s="1" t="inlineStr"/>
-      <c r="F57" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1463234/kerala-climate-resilient-agri-value-chain-modernization-kera-project-engagement-of-project-managemen</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" ht="80" customHeight="1">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B58" s="1" t="inlineStr">
-        <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Pipeline Condition Assessment for Urban Water Supply Networks in Rajasthan (58369-001)</t>
-        </is>
-      </c>
-      <c r="C58" s="1" t="inlineStr"/>
-      <c r="D58" s="1" t="inlineStr">
-        <is>
-          <t>Governance</t>
-        </is>
-      </c>
-      <c r="E58" s="1" t="inlineStr"/>
-      <c r="F58" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1583942/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-pipeline-condition-assessmen</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="80" customHeight="1">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B59" s="1" t="inlineStr">
-        <is>
-          <t>Call for External Collaborator – Extending Social Protection to Migrant Workers in an Irregular Situation (South Asia–GCC Corridor)</t>
-        </is>
-      </c>
-      <c r="C59" s="1" t="inlineStr"/>
-      <c r="D59" s="1" t="inlineStr">
-        <is>
-          <t>Safety</t>
-        </is>
-      </c>
-      <c r="E59" s="1" t="inlineStr"/>
-      <c r="F59" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1610212/call-for-external-collaborator-extending-social-protection-to-migrant-workers-in-an-irregular-situat</t>
-        </is>
-      </c>
-    </row>
-    <row r="60" ht="80" customHeight="1">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B60" s="1" t="inlineStr">
-        <is>
-          <t>RFP - Odia Annotation of Student Voice Recordings from Odisha</t>
-        </is>
-      </c>
-      <c r="C60" s="1" t="inlineStr"/>
-      <c r="D60" s="1" t="inlineStr">
-        <is>
-          <t>Learning</t>
-        </is>
-      </c>
-      <c r="E60" s="1" t="inlineStr"/>
-      <c r="F60" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1610092/rfp-odia-annotation-of-student-voice-recordings-from-odisha</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" ht="80" customHeight="1">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B61" s="1" t="inlineStr">
-        <is>
-          <t>RFP - English Annotation of Student Voice Recordings from Gujarat</t>
-        </is>
-      </c>
-      <c r="C61" s="1" t="inlineStr"/>
-      <c r="D61" s="1" t="inlineStr">
-        <is>
-          <t>Learning</t>
-        </is>
-      </c>
-      <c r="E61" s="1" t="inlineStr"/>
-      <c r="F61" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1610106/rfp-english-annotation-of-student-voice-recordings-from-gujarat</t>
+          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Fri Feb 27 04:10:12 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Skills: National ITI Upgradation Program - P507910</t>
+          <t>59395-001 - Support for Development and Implementation of the Private Capital Enabled Metric: Technical Assistance</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
@@ -540,7 +540,7 @@
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1425157/skills-national-iti-upgradation-program-p507910</t>
+          <t>https://www.developmentaid.org/tenders/view/1601673/59395-001-support-for-development-and-implementation-of-the-private-capital-enabled-metric-technical</t>
         </is>
       </c>
     </row>
@@ -552,19 +552,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: 04. SIUDP /DRY/THCC-01 - Design Build: Three Transit hubs cum community complex (THCCs) in Rangpo (Lot - 1), Ranipool (Lot - 2), and Pakyong (Lot - 3)</t>
+          <t>TA-6586 IND: Green Certification of Self Construction Housing (54340-001)</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1438614/57230-001-sikkim-integrated-urban-development-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1512890/ta-6586-ind-green-certification-of-self-construction-housing-54340-001</t>
         </is>
       </c>
     </row>
@@ -576,19 +576,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>LOAN 57262-001 IND: Assam Urban Sector Development Project - AUSDP/CMS/01 Project Management and Supervision Consultants (PMSC)</t>
+          <t>RFP - for Supply of Skill Lab Items</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1266713/loan-57262-001-ind-assam-urban-sector-development-project-ausdpcms01-project-management-and-supervis</t>
+          <t>https://www.developmentaid.org/tenders/view/1614712/rfp-for-supply-of-skill-lab-items</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Hiring of an Agency for Development of an Operational &amp; Implementation Plan for Solar Global Capability Center (GCC)</t>
+          <t>EoI - Construction &amp; Infrastructure Works – Schools Of Pali And Jodhpur Districts, Rajasthan</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
@@ -612,7 +612,7 @@
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614087/hiring-of-an-agency-for-development-of-an-operational-implementation-plan-for-solar-global-capabilit</t>
+          <t>https://www.developmentaid.org/tenders/view/1614736/eoi-construction-infrastructure-works-schools-of-pali-and-jodhpur-districts-rajasthan</t>
         </is>
       </c>
     </row>
@@ -624,19 +624,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>TA-9844 IND: Supporting Education and Skills Development Facility - Financial Management Specialist (53277-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB KOT ETTUMANOOR)</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613681/ta-9844-ind-supporting-education-and-skills-development-facility-financial-management-specialist-532</t>
+          <t>https://www.developmentaid.org/tenders/view/1095599/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-kot-ettumanoor-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -648,19 +648,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>RFP-011-IND-2026 - Agency for Development of a Gender-Responsive SDG framework</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR IRINJALAKKUDA)</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
+          <t>https://www.developmentaid.org/tenders/view/1212406/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-irinjalakkuda-procurement-pla</t>
         </is>
       </c>
     </row>
@@ -672,19 +672,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>TA-10416 IND: Promoting Disaster Risk Insurance (54081-001)</t>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613677/ta-10416-ind-promoting-disaster-risk-insurance-54081-001</t>
+          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
         </is>
       </c>
     </row>
@@ -696,19 +696,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB TSR KODUNGALLUR)</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1095626/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-kodungallur-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -720,19 +720,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Carpl.AI, Inc</t>
+          <t>P168633 - Kerala Solid Waste Management Project) - Procurement Plan (Ulb Mlp Thanur)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614052/carplai-inc</t>
+          <t>https://www.developmentaid.org/tenders/view/1095788/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-mlp-thanur-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -744,19 +744,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>RFQ - Final Evaluation of the UNESCO-Guerlain Women for Bees project</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR Guruvayoor)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614000/rfq-final-evaluation-of-the-unesco-guerlain-women-for-bees-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1202916/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-guruvayoor-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>TA-6742 REG: Building Coastal Resilience through Nature-Based and Integrated Solutions - Project Evaluation Specialist (54212-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB PGT C.T. MANGALAM)</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
@@ -780,7 +780,7 @@
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613663/ta-6742-reg-building-coastal-resilience-through-nature-based-and-integrated-solutions-project-evalua</t>
+          <t>https://www.developmentaid.org/tenders/view/1095582/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-ct-mangalam-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -792,19 +792,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB TSR CHALAKUDY)</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1108720/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-chalakudy-procurement-plan-en</t>
         </is>
       </c>
     </row>
@@ -816,19 +816,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
+          <t>Enabling Pathways for Long-term Low Emission Development Strategies for the Built Environment in India</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
+          <t>https://www.developmentaid.org/tenders/view/1614544/enabling-pathways-for-long-term-low-emission-development-strategies-for-the-built-environment-in-ind</t>
         </is>
       </c>
     </row>
@@ -840,19 +840,19 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4166 IND: Assam Skill University Project - CS11 Project Management Support for Capacity Development of Assam Civil Service (53277-002)</t>
+          <t>Skills: National ITI Upgradation Program - P507910</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1599394/loan-4166-ind-assam-skill-university-project-cs11-project-management-support-for-capacity-developmen</t>
+          <t>https://www.developmentaid.org/tenders/view/1425157/skills-national-iti-upgradation-program-p507910</t>
         </is>
       </c>
     </row>
@@ -864,19 +864,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: 04. SIUDP /DRY/THCC-01 - Design Build: Three Transit hubs cum community complex (THCCs) in Rangpo (Lot - 1), Ranipool (Lot - 2), and Pakyong (Lot - 3)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
+          <t>https://www.developmentaid.org/tenders/view/1438614/57230-001-sikkim-integrated-urban-development-project</t>
         </is>
       </c>
     </row>
@@ -888,19 +888,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
+          <t>LOAN 57262-001 IND: Assam Urban Sector Development Project - AUSDP/CMS/01 Project Management and Supervision Consultants (PMSC)</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1266713/loan-57262-001-ind-assam-urban-sector-development-project-ausdpcms01-project-management-and-supervis</t>
         </is>
       </c>
     </row>
@@ -912,19 +912,19 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
+          <t>Hiring of an Agency for Development of an Operational &amp; Implementation Plan for Solar Global Capability Center (GCC)</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1614087/hiring-of-an-agency-for-development-of-an-operational-implementation-plan-for-solar-global-capabilit</t>
         </is>
       </c>
     </row>
@@ -936,19 +936,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
+          <t>TA-9844 IND: Supporting Education and Skills Development Facility - Financial Management Specialist (53277-001)</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
+          <t>https://www.developmentaid.org/tenders/view/1613681/ta-9844-ind-supporting-education-and-skills-development-facility-financial-management-specialist-532</t>
         </is>
       </c>
     </row>
@@ -960,19 +960,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
+          <t>RFP-011-IND-2026 - Agency for Development of a Gender-Responsive SDG framework</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
+          <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
         </is>
       </c>
     </row>
@@ -984,19 +984,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
+          <t>TA-10416 IND: Promoting Disaster Risk Insurance (54081-001)</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
+          <t>https://www.developmentaid.org/tenders/view/1613677/ta-10416-ind-promoting-disaster-risk-insurance-54081-001</t>
         </is>
       </c>
     </row>
@@ -1008,19 +1008,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>
@@ -1032,19 +1032,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Evidence for AI in Health (EVAH)</t>
+          <t>Carpl.AI, Inc</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
+          <t>https://www.developmentaid.org/tenders/view/1614052/carplai-inc</t>
         </is>
       </c>
     </row>
@@ -1056,19 +1056,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
+          <t>RFQ - Final Evaluation of the UNESCO-Guerlain Women for Bees project</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
+          <t>https://www.developmentaid.org/tenders/view/1614000/rfq-final-evaluation-of-the-unesco-guerlain-women-for-bees-project</t>
         </is>
       </c>
     </row>
@@ -1080,19 +1080,19 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
+          <t>TA-6742 REG: Building Coastal Resilience through Nature-Based and Integrated Solutions - Project Evaluation Specialist (54212-001)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1613663/ta-6742-reg-building-coastal-resilience-through-nature-based-and-integrated-solutions-project-evalua</t>
         </is>
       </c>
     </row>
@@ -1104,19 +1104,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -1128,19 +1128,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -1152,19 +1152,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
+          <t>LOAN-4166 IND: Assam Skill University Project - CS11 Project Management Support for Capacity Development of Assam Civil Service (53277-002)</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
+          <t>https://www.developmentaid.org/tenders/view/1599394/loan-4166-ind-assam-skill-university-project-cs11-project-management-support-for-capacity-developmen</t>
         </is>
       </c>
     </row>
@@ -1176,19 +1176,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
         </is>
       </c>
     </row>
@@ -1200,19 +1200,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
+          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
+          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
         </is>
       </c>
     </row>
@@ -1224,19 +1224,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
+          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
+          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1248,19 +1248,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
+          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
+          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
         </is>
       </c>
     </row>
@@ -1272,19 +1272,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>Printing of Collaterals’ for State Refresher Training</t>
+          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
         </is>
       </c>
     </row>
@@ -1296,19 +1296,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
@@ -1332,7 +1332,7 @@
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1344,19 +1344,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+          <t>Evidence for AI in Health (EVAH)</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
         </is>
       </c>
     </row>
@@ -1368,19 +1368,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -1392,19 +1392,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
+          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
+          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
+          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
         </is>
       </c>
     </row>
@@ -1440,19 +1440,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
+          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
+          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
         </is>
       </c>
     </row>
@@ -1464,19 +1464,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
@@ -1500,7 +1500,7 @@
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1512,19 +1512,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
         </is>
       </c>
     </row>
@@ -1536,19 +1536,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>GEF SAGF IV: Growth Equity Fund</t>
+          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611328/gef-sagf-iv-growth-equity-fund</t>
+          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
         </is>
       </c>
     </row>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Consultancy, LiDAR survey of Greater Pamba River Basin, Digital Elevation Model, Flood Modelling and Flood Management Plan</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
@@ -1572,7 +1572,7 @@
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1538687/consultancy-lidar-survey-of-greater-pamba-river-basin-digital-elevation-model-flood-modelling-and-fl</t>
+          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
         </is>
       </c>
     </row>
@@ -1584,19 +1584,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Assam Disaster Resilient Hill Roads Development Project - P510002</t>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1453551/assam-disaster-resilient-hill-roads-development-project-p510002</t>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
         </is>
       </c>
     </row>
@@ -1608,19 +1608,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Assam School Education and Adolescent Wellbeing Project (ASAP) - P507865</t>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1462940/assam-school-education-and-adolescent-wellbeing-project-asap-p507865</t>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
         </is>
       </c>
     </row>
@@ -1632,19 +1632,19 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>Terms of Reference for hiring 'Event Management Agency'- PRS Project</t>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
       <c r="D50" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611188/terms-of-reference-for-hiring-event-management-agency-prs-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
         </is>
       </c>
     </row>
@@ -1656,19 +1656,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>Ausbau Erneuerbarer Energien / Expansion of renewable energies</t>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610971/ausbau-erneuerbarer-energien-expansion-of-renewable-energies</t>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
         </is>
       </c>
     </row>
@@ -1680,19 +1680,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>Klimaanpassung, Resilienz und Klimafinanzierung im ländlichen Indien / Climate adaptation, resilience and climate finance in rural India</t>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610948/klimaanpassung-resilienz-und-klimafinanzierung-im-landlichen-indien-climate-adaptation-resilience-an</t>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: MPKV Rahuri Development of Crop Weather Calendars, Spectral Libraries, and Irrigation Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA cluster of Maharashtra</t>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
@@ -1716,7 +1716,7 @@
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610861/maharashtra-project-on-climate-resilient-agriculture-phase-ii-mpkv-rahuri-development-of-crop-weathe</t>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: Development of Crop Weather Calendars and Databases to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in POCRA Clusters of Maharashtra</t>
+          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
@@ -1740,7 +1740,7 @@
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610860/maharashtra-project-on-climate-resilient-agriculture-phase-ii-development-of-crop-weather-calendars</t>
+          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
         </is>
       </c>
     </row>
@@ -1752,19 +1752,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>Integrated Project for Source Sustainability and Climate Resilient Rain-fed Agriculture in Himachal: Construction of Primary Water distribution   by laying HDPE/ GI pipes and installing pumps at different Locations in project G.P. 's of Sirmaur District</t>
+          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610843/integrated-project-for-source-sustainability-and-climate-resilient-rain-fed-agriculture-in-himachal</t>
+          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
         </is>
       </c>
     </row>
@@ -1776,19 +1776,67 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>Maharashtra Project on Climate Resilient Agriculture Phase - II: VNMKV Parbhani - Development of Crop Weather Calendars and Auto Agro-Advisories to Support Parcel-Level Real-Time Autonomous Agro-Advisory System for Farmers in PoCRA Clusters of Maharashtra</t>
+          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610856/maharashtra-project-on-climate-resilient-agriculture-phase-ii-vnmkv-parbhani-development-of-crop-wea</t>
+          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="80" customHeight="1">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr"/>
+      <c r="D57" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr"/>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="80" customHeight="1">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr"/>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr"/>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Sat Feb 28 03:51:23 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,19 +528,19 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>59395-001 - Support for Development and Implementation of the Private Capital Enabled Metric: Technical Assistance</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3413-IND: KEIIP (T2) - Package SD10T (Sewerage &amp; Drainage Network in Rania Box Catchment [Part of Wards 111, 112 and 113] in Borough XI) (56287-001)</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1601673/59395-001-support-for-development-and-implementation-of-the-private-capital-enabled-metric-technical</t>
+          <t>https://www.developmentaid.org/tenders/view/1615659/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -552,19 +552,19 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>TA-6586 IND: Green Certification of Self Construction Housing (54340-001)</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3689-IND: KEIIP (T3) - Package SD31L1 (Development of S&amp;D Network in Churial Extension PS Catchment and Diamond Park Catchment and Construction of pumping station [annexed] in Borough XVI [Part of Wards 124, 143 and 144]) (56287-001)</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety, Climate</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1512890/ta-6586-ind-green-certification-of-self-construction-housing-54340-001</t>
+          <t>https://www.developmentaid.org/tenders/view/1615657/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -576,19 +576,19 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>RFP - for Supply of Skill Lab Items</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3413-IND: KEIIP (T2) - Package SD11T (Sewerage &amp; Drainage Network in Vivekananda Road Catchment [Part of Wards 113 &amp; 114] and Construction of 1 Pumping Station in Borough XI) (56287-001)</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614712/rfp-for-supply-of-skill-lab-items</t>
+          <t>https://www.developmentaid.org/tenders/view/1615647/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -600,19 +600,19 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>EoI - Construction &amp; Infrastructure Works – Schools Of Pali And Jodhpur Districts, Rajasthan</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3689-IND: KEIIP (T3) - Package SD31R2 (Development of S&amp;D Network in Bakrahat Road Catchment [Ward 125] and Laying of RCC Sewer Line along Bakrahat Road and DH Road) (56287-001)</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Safety, Climate</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614736/eoi-construction-infrastructure-works-schools-of-pali-and-jodhpur-districts-rajasthan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615645/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -624,19 +624,19 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB KOT ETTUMANOOR)</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3689-IND: KEIIP (T3) - Package SD28 (Construction of WBSETCL Sewage Treatment Plant [45 MLD]) (56287-001)</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095599/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-kot-ettumanoor-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615644/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -648,19 +648,19 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR IRINJALAKKUDA)</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3689-IND: KEIIP (T3) - Package SD29 (Construction of Sewage Treatment Plant at Bank Plot [40 MLD]) (56287-001)</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1212406/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-irinjalakkuda-procurement-pla</t>
+          <t>https://www.developmentaid.org/tenders/view/1615642/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -672,19 +672,19 @@
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3413-IND: KEIIP (T2) - Package SD19 (Development of S&amp;D Network in Tolly's Nullah/Keorapukur Canal Sub-Basin in part of Wards 115 &amp; 122 including construction of SWF PS in Kudghat LS-5 &amp; augmentation of Keorapukur MPS) (56287-001)</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Learning, Safety, Climate</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
+          <t>https://www.developmentaid.org/tenders/view/1615639/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -696,19 +696,19 @@
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB TSR KODUNGALLUR)</t>
+          <t>Kolkata Municipal Corporation Sustainability, Hygiene, and Resilience (Sector) Project: Spillover works under L3689-IND: KEIIP (T3) - Package SD35 (Supply and Installation of Pumping Machineries for KEIIP) (56287-001)</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety, Climate</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095626/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-kodungallur-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615638/kolkata-municipal-corporation-sustainability-hygiene-and-resilience-sector-project-spillover-works-u</t>
         </is>
       </c>
     </row>
@@ -720,19 +720,19 @@
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>P168633 - Kerala Solid Waste Management Project) - Procurement Plan (Ulb Mlp Thanur)</t>
+          <t>TA-10548 IND: Supporting Institutional Knowledge and Capacity Development for Planning of Climate Resilient and Sustainable Projects - Financial Analysis Specialist - Preparation of the Industrial and Economic Corridor Sector Development Program in West Bengal (59006-001)</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095788/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-mlp-thanur-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615071/ta-10548-ind-supporting-institutional-knowledge-and-capacity-development-for-planning-of-climate-res</t>
         </is>
       </c>
     </row>
@@ -744,19 +744,19 @@
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR Guruvayoor)</t>
+          <t>P513815- Resilient Action for Development and Disaster Recovery Himachal Pradesh - Procurement Plan (Department of Revenue)</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E13" s="1" t="inlineStr"/>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1202916/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-guruvayoor-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615347/p513815-resilient-action-for-development-and-disaster-recovery-himachal-pradesh-procurement-plan-dep</t>
         </is>
       </c>
     </row>
@@ -768,19 +768,19 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB PGT C.T. MANGALAM)</t>
+          <t>Engagement of a Public Relations (PR) Agency on Retainer</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr"/>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1095582/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-ct-mangalam-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1615368/sow-engagement-of-a-public-relations-pr-agency-on-retainer</t>
         </is>
       </c>
     </row>
@@ -792,19 +792,19 @@
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>P168633- Kerala Solid Waste Management Project (ULB TSR CHALAKUDY)</t>
+          <t>RFP - External organization/agency to undertake documentation and process evaluation of the Gen Equal Fellowship Programme</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1108720/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-chalakudy-procurement-plan-en</t>
+          <t>https://www.developmentaid.org/tenders/view/1615372/rfp-external-organizationagency-to-undertake-documentation-and-process-evaluation-of-the-gen-equal-f</t>
         </is>
       </c>
     </row>
@@ -816,19 +816,19 @@
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Enabling Pathways for Long-term Low Emission Development Strategies for the Built Environment in India</t>
+          <t>Consultant – Endline Evaluation (Menstrual Health &amp; Hygiene Project)</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr"/>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614544/enabling-pathways-for-long-term-low-emission-development-strategies-for-the-built-environment-in-ind</t>
+          <t>https://www.developmentaid.org/tenders/view/1615395/consultant-endline-evaluation-menstrual-health-hygiene-project</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Skills: National ITI Upgradation Program - P507910</t>
+          <t>59395-001 - Support for Development and Implementation of the Private Capital Enabled Metric: Technical Assistance</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr"/>
@@ -852,7 +852,7 @@
       <c r="E17" s="1" t="inlineStr"/>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1425157/skills-national-iti-upgradation-program-p507910</t>
+          <t>https://www.developmentaid.org/tenders/view/1601673/59395-001-support-for-development-and-implementation-of-the-private-capital-enabled-metric-technical</t>
         </is>
       </c>
     </row>
@@ -864,19 +864,19 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>57230-001: Sikkim Integrated Urban Development Project: 04. SIUDP /DRY/THCC-01 - Design Build: Three Transit hubs cum community complex (THCCs) in Rangpo (Lot - 1), Ranipool (Lot - 2), and Pakyong (Lot - 3)</t>
+          <t>TA-6586 IND: Green Certification of Self Construction Housing (54340-001)</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1438614/57230-001-sikkim-integrated-urban-development-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1512890/ta-6586-ind-green-certification-of-self-construction-housing-54340-001</t>
         </is>
       </c>
     </row>
@@ -888,19 +888,19 @@
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>LOAN 57262-001 IND: Assam Urban Sector Development Project - AUSDP/CMS/01 Project Management and Supervision Consultants (PMSC)</t>
+          <t>RFP - for Supply of Skill Lab Items</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1266713/loan-57262-001-ind-assam-urban-sector-development-project-ausdpcms01-project-management-and-supervis</t>
+          <t>https://www.developmentaid.org/tenders/view/1614712/rfp-for-supply-of-skill-lab-items</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Hiring of an Agency for Development of an Operational &amp; Implementation Plan for Solar Global Capability Center (GCC)</t>
+          <t>EoI - Construction &amp; Infrastructure Works – Schools Of Pali And Jodhpur Districts, Rajasthan</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr"/>
@@ -924,7 +924,7 @@
       <c r="E20" s="1" t="inlineStr"/>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614087/hiring-of-an-agency-for-development-of-an-operational-implementation-plan-for-solar-global-capabilit</t>
+          <t>https://www.developmentaid.org/tenders/view/1614736/eoi-construction-infrastructure-works-schools-of-pali-and-jodhpur-districts-rajasthan</t>
         </is>
       </c>
     </row>
@@ -936,19 +936,19 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>TA-9844 IND: Supporting Education and Skills Development Facility - Financial Management Specialist (53277-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB KOT ETTUMANOOR)</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613681/ta-9844-ind-supporting-education-and-skills-development-facility-financial-management-specialist-532</t>
+          <t>https://www.developmentaid.org/tenders/view/1095599/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-kot-ettumanoor-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -960,19 +960,19 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>RFP-011-IND-2026 - Agency for Development of a Gender-Responsive SDG framework</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR IRINJALAKKUDA)</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
+          <t>https://www.developmentaid.org/tenders/view/1212406/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-irinjalakkuda-procurement-pla</t>
         </is>
       </c>
     </row>
@@ -984,19 +984,19 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>TA-10416 IND: Promoting Disaster Risk Insurance (54081-001)</t>
+          <t>P178418 - Tripura Rural Economic Growth and Service Delivery Project - Procurement Plan (Public Works Department, Roads and Bridges)</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613677/ta-10416-ind-promoting-disaster-risk-insurance-54081-001</t>
+          <t>https://www.developmentaid.org/tenders/view/978729/india-south-asia-p178418-tripura-rural-economic-growth-and-service-delivery-project-public-works-dep</t>
         </is>
       </c>
     </row>
@@ -1008,19 +1008,19 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB TSR KODUNGALLUR)</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1095626/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-kodungallur-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1032,19 +1032,19 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Carpl.AI, Inc</t>
+          <t>P168633 - Kerala Solid Waste Management Project) - Procurement Plan (Ulb Mlp Thanur)</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614052/carplai-inc</t>
+          <t>https://www.developmentaid.org/tenders/view/1095788/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-mlp-thanur-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1056,19 +1056,19 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>RFQ - Final Evaluation of the UNESCO-Guerlain Women for Bees project</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB TSR Guruvayoor)</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1614000/rfq-final-evaluation-of-the-unesco-guerlain-women-for-bees-project</t>
+          <t>https://www.developmentaid.org/tenders/view/1202916/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-guruvayoor-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>TA-6742 REG: Building Coastal Resilience through Nature-Based and Integrated Solutions - Project Evaluation Specialist (54212-001)</t>
+          <t>P168633- Kerala Solid Waste Management Project - Procurement Plan (ULB PGT C.T. MANGALAM)</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr"/>
@@ -1092,7 +1092,7 @@
       <c r="E27" s="1" t="inlineStr"/>
       <c r="F27" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613663/ta-6742-reg-building-coastal-resilience-through-nature-based-and-integrated-solutions-project-evalua</t>
+          <t>https://www.developmentaid.org/tenders/view/1095582/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-pgt-ct-mangalam-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1104,19 +1104,19 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
+          <t>P168633- Kerala Solid Waste Management Project (ULB TSR CHALAKUDY)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr"/>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
+          <t>https://www.developmentaid.org/tenders/view/1108720/india-south-asia-p168633-kerala-solid-waste-management-project-ulb-tsr-chalakudy-procurement-plan-en</t>
         </is>
       </c>
     </row>
@@ -1128,19 +1128,19 @@
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
+          <t>Enabling Pathways for Long-term Low Emission Development Strategies for the Built Environment in India</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr"/>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Climate</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr"/>
       <c r="F29" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
+          <t>https://www.developmentaid.org/tenders/view/1614544/enabling-pathways-for-long-term-low-emission-development-strategies-for-the-built-environment-in-ind</t>
         </is>
       </c>
     </row>
@@ -1152,19 +1152,19 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>LOAN-4166 IND: Assam Skill University Project - CS11 Project Management Support for Capacity Development of Assam Civil Service (53277-002)</t>
+          <t>Skills: National ITI Upgradation Program - P507910</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr"/>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr"/>
       <c r="F30" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1599394/loan-4166-ind-assam-skill-university-project-cs11-project-management-support-for-capacity-developmen</t>
+          <t>https://www.developmentaid.org/tenders/view/1425157/skills-national-iti-upgradation-program-p507910</t>
         </is>
       </c>
     </row>
@@ -1176,19 +1176,19 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
+          <t>57230-001: Sikkim Integrated Urban Development Project: 04. SIUDP /DRY/THCC-01 - Design Build: Three Transit hubs cum community complex (THCCs) in Rangpo (Lot - 1), Ranipool (Lot - 2), and Pakyong (Lot - 3)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr"/>
       <c r="F31" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
+          <t>https://www.developmentaid.org/tenders/view/1438614/57230-001-sikkim-integrated-urban-development-project</t>
         </is>
       </c>
     </row>
@@ -1200,19 +1200,19 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
+          <t>LOAN 57262-001 IND: Assam Urban Sector Development Project - AUSDP/CMS/01 Project Management and Supervision Consultants (PMSC)</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr"/>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
+          <t>https://www.developmentaid.org/tenders/view/1266713/loan-57262-001-ind-assam-urban-sector-development-project-ausdpcms01-project-management-and-supervis</t>
         </is>
       </c>
     </row>
@@ -1224,19 +1224,19 @@
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
+          <t>Hiring of an Agency for Development of an Operational &amp; Implementation Plan for Solar Global Capability Center (GCC)</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr"/>
       <c r="F33" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
+          <t>https://www.developmentaid.org/tenders/view/1614087/hiring-of-an-agency-for-development-of-an-operational-implementation-plan-for-solar-global-capabilit</t>
         </is>
       </c>
     </row>
@@ -1248,19 +1248,19 @@
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
+          <t>TA-9844 IND: Supporting Education and Skills Development Facility - Financial Management Specialist (53277-001)</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr"/>
       <c r="D34" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E34" s="1" t="inlineStr"/>
       <c r="F34" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
+          <t>https://www.developmentaid.org/tenders/view/1613681/ta-9844-ind-supporting-education-and-skills-development-facility-financial-management-specialist-532</t>
         </is>
       </c>
     </row>
@@ -1272,19 +1272,19 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
+          <t>RFP-011-IND-2026 - Agency for Development of a Gender-Responsive SDG framework</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr"/>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Learning, Safety</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr"/>
       <c r="F35" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
+          <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
         </is>
       </c>
     </row>
@@ -1296,19 +1296,19 @@
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
+          <t>TA-10416 IND: Promoting Disaster Risk Insurance (54081-001)</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr"/>
       <c r="D36" s="1" t="inlineStr">
         <is>
-          <t>Governance, Safety</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E36" s="1" t="inlineStr"/>
       <c r="F36" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
+          <t>https://www.developmentaid.org/tenders/view/1613677/ta-10416-ind-promoting-disaster-risk-insurance-54081-001</t>
         </is>
       </c>
     </row>
@@ -1320,19 +1320,19 @@
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
+          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr"/>
       <c r="D37" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr"/>
       <c r="F37" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>
@@ -1344,19 +1344,19 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Evidence for AI in Health (EVAH)</t>
+          <t>Carpl.AI, Inc</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr"/>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Learning, Safety</t>
+          <t>Learning</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr"/>
       <c r="F38" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
+          <t>https://www.developmentaid.org/tenders/view/1614052/carplai-inc</t>
         </is>
       </c>
     </row>
@@ -1368,19 +1368,19 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
+          <t>RFQ - Final Evaluation of the UNESCO-Guerlain Women for Bees project</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr"/>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr"/>
       <c r="F39" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
+          <t>https://www.developmentaid.org/tenders/view/1614000/rfq-final-evaluation-of-the-unesco-guerlain-women-for-bees-project</t>
         </is>
       </c>
     </row>
@@ -1392,19 +1392,19 @@
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
+          <t>TA-6742 REG: Building Coastal Resilience through Nature-Based and Integrated Solutions - Project Evaluation Specialist (54212-001)</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr"/>
       <c r="D40" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr"/>
       <c r="F40" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
+          <t>https://www.developmentaid.org/tenders/view/1613663/ta-6742-reg-building-coastal-resilience-through-nature-based-and-integrated-solutions-project-evalua</t>
         </is>
       </c>
     </row>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
+          <t>Call for External Collaborator – The ILO project ‘Strengthening Labour Dispute Resolution in Tamil Nadu’s Electronics Manufacturing Sector’ invites applications from consultants to support develop &amp; deliver capacity building programme for social partners</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr"/>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr"/>
       <c r="F41" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
+          <t>https://www.developmentaid.org/tenders/view/1610322/call-for-external-collaborator-the-ilo-project-strengthening-labour-dispute-resolution-in-tamil-nadu</t>
         </is>
       </c>
     </row>
@@ -1440,19 +1440,19 @@
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
+          <t>P170873- Second Dam Rehabilitation and Improvement Project - Procurement Plan (Bhakra Beas Management Board)</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr"/>
       <c r="F42" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
+          <t>https://www.developmentaid.org/tenders/view/1611929/p170873-second-dam-rehabilitation-and-improvement-project-procurement-plan-bhakra-beas-management-bo</t>
         </is>
       </c>
     </row>
@@ -1464,19 +1464,19 @@
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
+          <t>LOAN-4166 IND: Assam Skill University Project - CS11 Project Management Support for Capacity Development of Assam Civil Service (53277-002)</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr"/>
       <c r="D43" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Governance, Learning</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr"/>
       <c r="F43" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
+          <t>https://www.developmentaid.org/tenders/view/1599394/loan-4166-ind-assam-skill-university-project-cs11-project-management-support-for-capacity-developmen</t>
         </is>
       </c>
     </row>
@@ -1488,19 +1488,19 @@
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
+          <t>56283-002 - Climate Resilient Brahmaputra Integrated Flood and Riverbank Erosion Risk Management Project in Assam - Additional Financing</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr"/>
       <c r="D44" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr"/>
       <c r="F44" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
+          <t>https://www.developmentaid.org/tenders/view/1543921/56283-002-climate-resilient-brahmaputra-integrated-flood-and-riverbank-erosion-risk-management-proje</t>
         </is>
       </c>
     </row>
@@ -1512,19 +1512,19 @@
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
+          <t>59459-001 - Building Knowledge-Based Innovative Solutions for Sustainable and Clean Energy in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr"/>
       <c r="D45" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr"/>
       <c r="F45" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
+          <t>https://www.developmentaid.org/tenders/view/1584578/59459-001-building-knowledge-based-innovative-solutions-for-sustainable-and-clean-energy-in-asia-and</t>
         </is>
       </c>
     </row>
@@ -1536,19 +1536,19 @@
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
+          <t>59305-001 - Catalyzing Sustainable Transport Initiatives in Asia and the Pacific: Technical Assistance</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr"/>
       <c r="D46" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning</t>
+          <t>Safety</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr"/>
       <c r="F46" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
+          <t>https://www.developmentaid.org/tenders/view/1552965/59305-001-catalyzing-sustainable-transport-initiatives-in-asia-and-the-pacific-technical-assistance</t>
         </is>
       </c>
     </row>
@@ -1560,19 +1560,19 @@
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
+          <t>59388-001 - Accelerating and Sustaining Universal Health Coverage (UHC) through UHC Practitioners and Experts knowledge Exchange and Resources (UHC PEERS) Network: Technical Assistance</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr"/>
       <c r="D47" s="1" t="inlineStr">
         <is>
-          <t>Governance, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr"/>
       <c r="F47" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
+          <t>https://www.developmentaid.org/tenders/view/1572727/59388-001-accelerating-and-sustaining-universal-health-coverage-uhc-through-uhc-practitioners-and-ex</t>
         </is>
       </c>
     </row>
@@ -1584,19 +1584,19 @@
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>Printing of Collaterals’ for State Refresher Training</t>
+          <t>59384-001 - Strengthening Quality, Sustainability and Value for Money through Implementation of the 2026 Procurement Directive for ADB Borrowers: Technical Assistance</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr"/>
       <c r="D48" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E48" s="1" t="inlineStr"/>
       <c r="F48" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+          <t>https://www.developmentaid.org/tenders/view/1613609/59384-001-strengthening-quality-sustainability-and-value-for-money-through-implementation-of-the-202</t>
         </is>
       </c>
     </row>
@@ -1608,19 +1608,19 @@
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+          <t>Onboarding of a Consultancy / Research Firm for Economic Impact Analysis of Public Health Supply Chain Strengthening</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr"/>
       <c r="D49" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance, Safety</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr"/>
       <c r="F49" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+          <t>https://www.developmentaid.org/tenders/view/1613408/rfp-2026-in-01-agency-for-economic-impact-analysis</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+          <t>57133-001 - Sustainable and Inclusive Tourism Development Project in Himachal Pradesh: Procurement Plan</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr"/>
@@ -1644,7 +1644,7 @@
       <c r="E50" s="1" t="inlineStr"/>
       <c r="F50" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+          <t>https://www.developmentaid.org/tenders/view/1377325/57133-001-sustainable-and-inclusive-tourism-development-project-in-himachal-pradesh-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1656,19 +1656,19 @@
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+          <t>Evidence for AI in Health (EVAH)</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr"/>
       <c r="D51" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Learning, Safety</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr"/>
       <c r="F51" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+          <t>https://www.developmentaid.org/tenders/view/1613299/evidence-for-ai-in-health-evah</t>
         </is>
       </c>
     </row>
@@ -1680,19 +1680,19 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+          <t>P179749- Uttarakhand Disaster Preparedness and Resilience Project - Procurement Plan (PIU- Rural Works Department)</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr"/>
       <c r="D52" s="1" t="inlineStr">
         <is>
-          <t>Governance, Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr"/>
       <c r="F52" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+          <t>https://www.developmentaid.org/tenders/view/1485844/p179749-uttarakhand-disaster-preparedness-and-resilience-project-procurement-plan-piu-rural-works-de</t>
         </is>
       </c>
     </row>
@@ -1704,19 +1704,19 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+          <t>P178581 - Assam Resilient Rural Bridges Program - Procurement Plan (Public Works Roads Department, Assam)</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr"/>
       <c r="D53" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E53" s="1" t="inlineStr"/>
       <c r="F53" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
+          <t>https://www.developmentaid.org/tenders/view/1189984/india-south-asia-p178581-assam-resilient-rural-bridges-program-procurement-plan</t>
         </is>
       </c>
     </row>
@@ -1728,19 +1728,19 @@
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>P179189- Tamil Nadu Climate Resilient Urban Development Program - Procurement Plan (Tamil Nadu Urban Infrastructure Financial Services Limited)</t>
+          <t>P180932 - Strengthening Coastal Resilience and the Economy - Procurement Plan (Tamil Nadu Green Climate Company (TNGCC))</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
       <c r="D54" s="1" t="inlineStr">
         <is>
-          <t>Learning, Climate</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr"/>
       <c r="F54" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1189983/india-south-asia-p179189-tamil-nadu-climate-resilient-urban-development-program-tamil-nadu-urban-inf</t>
+          <t>https://www.developmentaid.org/tenders/view/1326097/india-south-asia-p180932-strengthening-coastal-resilience-and-the-economy-tamil-nadu-green-climate-c</t>
         </is>
       </c>
     </row>
@@ -1752,19 +1752,19 @@
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>TA-10446 REG: Improving Governance for Urban and Water Service Providers - Capacity Building Coordination Specialist (Internationl) (58369-001)</t>
+          <t>P179935 - Enhancing Landscape and Ecosystem Management Project - Procurement Plan (Society for Climate Resilient Agriculture in Nagaland)</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr"/>
       <c r="D55" s="1" t="inlineStr">
         <is>
-          <t>Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr"/>
       <c r="F55" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611636/ta-10446-reg-improving-governance-for-urban-and-water-service-providers-capacity-building-coordinati</t>
+          <t>https://www.developmentaid.org/tenders/view/1145475/india-south-asia-p179935-enhancing-landscape-and-ecosystem-management-project-society-for-climate-re</t>
         </is>
       </c>
     </row>
@@ -1776,19 +1776,19 @@
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>Procurement of Laboratory Equipment &amp; Consumables for AMR laboratories in India, including delivery, installation, assembly, commissioning of equipment at the installation site and training services</t>
+          <t>P163533- Odisha Integrated Irrigation Project for Climate Resilient Agriculture - Procurement Plan (Odisha community Tank Development and Management Society)</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr"/>
       <c r="D56" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance, Learning, Climate</t>
         </is>
       </c>
       <c r="E56" s="1" t="inlineStr"/>
       <c r="F56" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1604282/procurement-of-laboratory-equipment-consumables-for-amr-laboratories-in-india-including-delivery-ins</t>
+          <t>https://www.developmentaid.org/tenders/view/484340/india-south-asia-p163533-odisha-integrated-irrigation-project-for-climate-resilient-agriculture-proc</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>Non-Profit Organizations for Community Mobilization, Capacity Building, Training, Stakeholder Engagement, Convergence, Data Collection and Project Documentation</t>
+          <t>TA-6822 IND: Support for Strengthening Multimodal and Integrated Logistics Ecosystem - Development of Sectoral Plan for Efficient Logistics (SPEL) for Wheat, Rice and Millets under Public Distribution System - Agri-market Assessment Expert (55154-002)</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr"/>
@@ -1812,7 +1812,7 @@
       <c r="E57" s="1" t="inlineStr"/>
       <c r="F57" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611610/community-mobilizationawareness-capacity-buildingdata-collectionconvergence</t>
+          <t>https://www.developmentaid.org/tenders/view/1607893/ta-6822-ind-support-for-strengthening-multimodal-and-integrated-logistics-ecosystem-development-of-s</t>
         </is>
       </c>
     </row>
@@ -1824,19 +1824,211 @@
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>RFP-009-IND-2026 RFP for Dissemination and Uptake of the Study ‘AI for Justice</t>
+          <t>RFP - Final Evaluation of the Bhoomi Ka Programme</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr"/>
       <c r="D58" s="1" t="inlineStr">
         <is>
-          <t>Learning</t>
+          <t>Governance</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr"/>
       <c r="F58" s="1" t="inlineStr">
         <is>
-          <t>https://www.developmentaid.org/tenders/view/1611609/rfp-009-ind-2026-rfp-for-dissemination-and-uptake-of-the-study-ai-for-justice</t>
+          <t>https://www.developmentaid.org/tenders/view/1612729/rfp-final-evaluation-of-the-bhoomi-ka-programme</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="80" customHeight="1">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>RFP- for Hiring a Resource Person/Agency Development of MEAL Questionnaires and Processes for CommCare Tool</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr"/>
+      <c r="D59" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr"/>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612750/rfp-for-hiring-a-resource-personagency-development-of-meal-questionnaires-and-processes-for-commcare</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="80" customHeight="1">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project - Procurement Plan (State Project Management Unit (Kerala))</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr"/>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Climate</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr"/>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612677/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-procurement-plan-state</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" ht="80" customHeight="1">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>Printing of Collaterals’ for State Refresher Training</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr"/>
+      <c r="D61" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E61" s="1" t="inlineStr"/>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612222/printing-of-collaterals-for-state-refresher-training</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="80" customHeight="1">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>Deutsch#indisches Programm für Green Skills IGGSP / German-Indian Green Skills Programme IGGSP</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr"/>
+      <c r="D62" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr"/>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612146/deutschindisches-programm-fur-green-skills-iggsp-german-indian-green-skills-programme-iggsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" ht="80" customHeight="1">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>EoI – Mobile Medical Units, Ai-Enabled Tb Screening &amp; Supply Of Medical And Nutritional Support</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr"/>
+      <c r="D63" s="1" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+      <c r="E63" s="1" t="inlineStr"/>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612050/eoi-mobile-medical-units-ai-enabled-tb-screening-supply-of-medical-and-nutritional-support</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="80" customHeight="1">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Onboarding Agency for Revamping Assam LMIS Dashboard</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr"/>
+      <c r="D64" s="1" t="inlineStr">
+        <is>
+          <t>Governance</t>
+        </is>
+      </c>
+      <c r="E64" s="1" t="inlineStr"/>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612059/rfp-onboarding-agency-for-revamping-assam-lmis-dashboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="80" customHeight="1">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>RFP - Long-term Monitoring &amp; Evaluation (M&amp;E) Partnership for Environment and Education Programme in MP, MH and TG</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr"/>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Governance, Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr"/>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1612065/rfp-long-term-monitoring-evaluation-me-partnership-for-environment-and-education-programme-in-mp-mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="80" customHeight="1">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>DevelopmentAid</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>P178254- Kerala Climate Resilient Agri- Value Chain Modernization (KERA) Project (Agriculture Development and Farmers’ Welfare Department.)</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr"/>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Learning, Climate</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr"/>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>https://www.developmentaid.org/tenders/view/1393178/p178254-kerala-climate-resilient-agri-value-chain-modernization-kera-project-agriculture-development</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Combined.xlsx [Mon Mar  2 04:10:17 UTC 2026]
</commit_message>
<xml_diff>
--- a/output/Combined.xlsx
+++ b/output/Combined.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,7 +766,7 @@
       <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr"/>
@@ -790,7 +790,7 @@
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr"/>
@@ -814,7 +814,7 @@
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr"/>
@@ -838,7 +838,7 @@
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr"/>
@@ -862,7 +862,7 @@
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr"/>
@@ -886,7 +886,7 @@
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr"/>
@@ -910,7 +910,7 @@
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
@@ -934,7 +934,7 @@
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Safety, Climate, Governance</t>
+          <t>Safety, Governance, Climate</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
@@ -1126,7 +1126,7 @@
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr"/>
@@ -1150,7 +1150,7 @@
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr"/>
@@ -1198,7 +1198,7 @@
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr"/>
@@ -1222,7 +1222,7 @@
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr"/>
@@ -1246,7 +1246,7 @@
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr"/>
@@ -1270,7 +1270,7 @@
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr"/>
@@ -1294,7 +1294,7 @@
       <c r="C25" s="1" t="inlineStr"/>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>Climate, Governance</t>
+          <t>Governance, Climate</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr"/>
@@ -1433,34 +1433,6 @@
       <c r="F30" s="1" t="inlineStr">
         <is>
           <t>https://www.developmentaid.org/tenders/view/1614135/rfp-011-ind-2026-agency-for-development-of-a-gender-responsive-sdg-framework</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="95" customHeight="1">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>DevelopmentAid</t>
-        </is>
-      </c>
-      <c r="B31" s="1" t="inlineStr">
-        <is>
-          <t>RFP for for Developing Integrated One Health Portal for enhanced collaborative Surveillance</t>
-        </is>
-      </c>
-      <c r="C31" s="1" t="inlineStr"/>
-      <c r="D31" s="1" t="inlineStr">
-        <is>
-          <t>Safety</t>
-        </is>
-      </c>
-      <c r="E31" s="1" t="inlineStr">
-        <is>
-          <t>Mar 8, 2026</t>
-        </is>
-      </c>
-      <c r="F31" s="1" t="inlineStr">
-        <is>
-          <t>https://www.developmentaid.org/tenders/view/1607851/rfp-for-for-developing-integrated-one-health-portal-for-enhanced-collaborative-s</t>
         </is>
       </c>
     </row>

</xml_diff>